<commit_message>
added rcs to non-linear variables for logreg models, removed feature selection methods, removed interaction analysis, added age at t1d diagnosis variable to models
</commit_message>
<xml_diff>
--- a/Diabetic_complications_tables.xlsx
+++ b/Diabetic_complications_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paultran/Box/Students/T1D_complications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E6E1E0-DC6E-7344-855F-4C2BF446327B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F56D24-0AEC-804E-9822-79F326C19343}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17220" yWindow="1600" windowWidth="14180" windowHeight="16940" firstSheet="2" activeTab="5" xr2:uid="{D1842A1F-FBE3-7248-88B5-8CE7C8CE474E}"/>
+    <workbookView xWindow="17080" yWindow="1180" windowWidth="16520" windowHeight="16940" firstSheet="5" activeTab="7" xr2:uid="{D1842A1F-FBE3-7248-88B5-8CE7C8CE474E}"/>
   </bookViews>
   <sheets>
     <sheet name="table 1 raw" sheetId="5" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="table 3" sheetId="11" r:id="rId6"/>
     <sheet name="interaction improvement" sheetId="12" r:id="rId7"/>
     <sheet name="lrm mods odds ratios" sheetId="14" r:id="rId8"/>
+    <sheet name="lrm mods validity" sheetId="15" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="297">
   <si>
     <t>Peripheral_Neuropathy3</t>
   </si>
@@ -751,109 +752,178 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Adjusted</t>
-  </si>
-  <si>
-    <t>to:</t>
-  </si>
-  <si>
-    <t>Dr_Age=25.38998</t>
-  </si>
-  <si>
-    <t>Dur=10.88318</t>
-  </si>
-  <si>
-    <t>n=1335</t>
-  </si>
-  <si>
-    <t>absolute</t>
-  </si>
-  <si>
-    <t>error=0.024</t>
-  </si>
-  <si>
-    <t>squared</t>
-  </si>
-  <si>
-    <t>error=0.00117</t>
-  </si>
-  <si>
-    <t>Quantile</t>
-  </si>
-  <si>
-    <t>of</t>
-  </si>
-  <si>
-    <t>error=0.061</t>
-  </si>
-  <si>
-    <t>n=1332</t>
-  </si>
-  <si>
-    <t>error=0.012</t>
-  </si>
-  <si>
-    <t>error=0.00042</t>
-  </si>
-  <si>
-    <t>error=0.023</t>
-  </si>
-  <si>
-    <t>n=1337</t>
-  </si>
-  <si>
-    <t>error=0.035</t>
-  </si>
-  <si>
-    <t>error=0.00262</t>
-  </si>
-  <si>
-    <t>error=0.076</t>
-  </si>
-  <si>
-    <t>n=1334</t>
-  </si>
-  <si>
-    <t>error=0.011</t>
-  </si>
-  <si>
-    <t>error=0.00062</t>
-  </si>
-  <si>
-    <t>error=0.022</t>
-  </si>
-  <si>
-    <t>error=0.014</t>
-  </si>
-  <si>
-    <t>error=0.00045</t>
-  </si>
-  <si>
-    <t>error=0.04</t>
-  </si>
-  <si>
-    <t>error=0.007</t>
-  </si>
-  <si>
-    <t>error=0.00016</t>
-  </si>
-  <si>
-    <t>error=0.019</t>
-  </si>
-  <si>
-    <t>error=0.013</t>
-  </si>
-  <si>
-    <t>error=4e-04</t>
-  </si>
-  <si>
-    <t>error=0.025</t>
-  </si>
-  <si>
-    <t>error=0.004</t>
-  </si>
-  <si>
-    <t>error=8e-05</t>
+    <t>index.orig</t>
+  </si>
+  <si>
+    <t>training</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>optimism</t>
+  </si>
+  <si>
+    <t>index.corrected</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Dxy</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>Emax</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>gp</t>
+  </si>
+  <si>
+    <t>Divergence</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>singularity</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>samples</t>
+  </si>
+  <si>
+    <t>C-index = 0.5 * ( Dxy + 1 )</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>n=1335   Mean absolute error=0.009   Mean squared error=0.00023</t>
+  </si>
+  <si>
+    <t>0.9 Quantile of absolute error=0.029</t>
+  </si>
+  <si>
+    <t>Divergence or singularity in 34 samples</t>
+  </si>
+  <si>
+    <t>n=1332   Mean absolute error=0.004   Mean squared error=4e-05</t>
+  </si>
+  <si>
+    <t>0.9 Quantile of absolute error=0.01</t>
+  </si>
+  <si>
+    <t>n=1337   Mean absolute error=0.006   Mean squared error=0.00011</t>
+  </si>
+  <si>
+    <t>0.9 Quantile of absolute error=0.014</t>
+  </si>
+  <si>
+    <t>n=1334   Mean absolute error=0.004   Mean squared error=8e-05</t>
+  </si>
+  <si>
+    <t>0.9 Quantile of absolute error=0.009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 1: Peripheral_Neuropathy3 ~ Autonomic_Neuropathy3 + DM_Retinopathy3 + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    DM_Nephropathy3 + Sex + Smoking + HTN3 + Dyslipidemia3 + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dr_Age + Dx_Age + Dur + Hemoglobin + Albumin + LDL + Total_Cholesterol + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Triglycerides + HDL + avg.BUN + avg.Creatinine + avg.Systolic + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    avg.diastolic + avg.MicroAlb + ACR + AvgA1c + SDA1c + HbA1c_3.1 + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Max_HbA1c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 2: Peripheral_Neuropathy3 ~ rcs(Dr_Age, 3) + Dur + avg.Systolic + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    rcs(Dx_Age, 5) + rcs(AvgA1c, 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L.R. Chisq       d.f.          P </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  184.7573    16.0000     0.0000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 1: Autonomic_Neuropathy3 ~ Peripheral_Neuropathy3 + DM_Retinopathy3 + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 2: Autonomic_Neuropathy3 ~ rcs(Dr_Age, 3) + Dur + rcs(Dx_Age, 5) + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    avg.Systolic + rcs(AvgA1c, 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> L.R. Chisq        d.f.           P </t>
+  </si>
+  <si>
+    <t xml:space="preserve">31.63431939 16.00000000  0.01115383 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 1: DM_Retinopathy3 ~ Autonomic_Neuropathy3 + Peripheral_Neuropathy3 + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 2: DM_Retinopathy3 ~ rcs(Dr_Age, 3) + rcs(Dur, 3) + rcs(Dx_Age, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    5) + avg.Systolic + rcs(AvgA1c, 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  349.9209    15.0000     0.0000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 1: DM_Nephropathy3 ~ Autonomic_Neuropathy3 + Peripheral_Neuropathy3 + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    DM_Retinopathy3 + Sex + Smoking + HTN3 + Dyslipidemia3 + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 2: DM_Nephropathy3 ~ rcs(Dr_Age, 3) + Dur + rcs(Dx_Age, 5) + avg.Systolic + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    rcs(AvgA1c, 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  L.R. Chisq         d.f.            P </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.634497e+01 1.600000e+01 2.134086e-06 </t>
   </si>
 </sst>
 </file>
@@ -864,7 +934,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -927,6 +997,13 @@
       <name val="Courier New"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -984,7 +1061,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1068,6 +1145,10 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1086,10 +1167,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6000,26 +6078,26 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="23"/>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37" t="s">
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37" t="s">
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
     </row>
     <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="23" t="s">
@@ -8989,13 +9067,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F9B48A-01B3-4443-ACA5-8A19E219CDB7}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -9018,26 +9108,26 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="41" t="s">
+      <c r="F2" s="46"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="41" t="s">
+      <c r="I2" s="46"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="42"/>
-      <c r="M2" s="40"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="44"/>
       <c r="N2" s="12"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -9112,7 +9202,7 @@
         <v>205</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L4" s="13" t="s">
         <v>205</v>
@@ -9135,21 +9225,19 @@
       <c r="D5" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>206</v>
-      </c>
+      <c r="E5" s="16"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13" t="s">
         <v>206</v>
       </c>
       <c r="H5" s="16"/>
-      <c r="I5" s="13"/>
+      <c r="I5" s="13" t="s">
+        <v>206</v>
+      </c>
       <c r="J5" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="K5" s="16" t="s">
-        <v>206</v>
-      </c>
+      <c r="K5" s="16"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13" t="s">
         <v>206</v>
@@ -9165,9 +9253,7 @@
       <c r="D6" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>206</v>
-      </c>
+      <c r="E6" s="16"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13" t="s">
         <v>206</v>
@@ -9181,10 +9267,10 @@
       <c r="J6" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="16"/>
+      <c r="L6" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="L6" s="13"/>
       <c r="M6" s="13" t="s">
         <v>206</v>
       </c>
@@ -9200,10 +9286,10 @@
       <c r="E7" s="16"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="16"/>
+      <c r="I7" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="I7" s="13"/>
       <c r="J7" s="13"/>
       <c r="K7" s="16"/>
       <c r="L7" s="13"/>
@@ -9229,12 +9315,14 @@
       <c r="H8" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="I8" s="13"/>
+      <c r="I8" s="13" t="s">
+        <v>205</v>
+      </c>
       <c r="J8" s="13"/>
-      <c r="K8" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="L8" s="13"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="13" t="s">
+        <v>205</v>
+      </c>
       <c r="M8" s="13"/>
       <c r="N8" s="33"/>
     </row>
@@ -9249,20 +9337,18 @@
         <v>205</v>
       </c>
       <c r="D9" s="13"/>
-      <c r="E9" s="16" t="s">
-        <v>205</v>
-      </c>
+      <c r="E9" s="16"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
-      <c r="H9" s="16" t="s">
-        <v>205</v>
-      </c>
+      <c r="H9" s="16"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="L9" s="13"/>
+      <c r="L9" s="13" t="s">
+        <v>205</v>
+      </c>
       <c r="M9" s="13"/>
       <c r="N9" s="33"/>
     </row>
@@ -9270,9 +9356,7 @@
       <c r="A10" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>205</v>
-      </c>
+      <c r="B10" s="16"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="16"/>
@@ -9281,11 +9365,11 @@
       <c r="H10" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="I10" s="13"/>
+      <c r="I10" s="13" t="s">
+        <v>205</v>
+      </c>
       <c r="J10" s="13"/>
-      <c r="K10" s="16" t="s">
-        <v>206</v>
-      </c>
+      <c r="K10" s="16"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
       <c r="N10" s="33"/>
@@ -9294,25 +9378,25 @@
       <c r="A11" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>205</v>
-      </c>
+      <c r="B11" s="16"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="16" t="s">
-        <v>205</v>
-      </c>
+      <c r="E11" s="16"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="I11" s="13"/>
+      <c r="I11" s="13" t="s">
+        <v>205</v>
+      </c>
       <c r="J11" s="13"/>
       <c r="K11" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="L11" s="13"/>
+        <v>205</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>205</v>
+      </c>
       <c r="M11" s="13"/>
       <c r="N11" s="33"/>
     </row>
@@ -9327,11 +9411,11 @@
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="16"/>
-      <c r="I12" s="13"/>
+      <c r="I12" s="13" t="s">
+        <v>206</v>
+      </c>
       <c r="J12" s="13"/>
-      <c r="K12" s="16" t="s">
-        <v>205</v>
-      </c>
+      <c r="K12" s="16"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="33"/>
@@ -9345,18 +9429,18 @@
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="16" t="s">
-        <v>205</v>
-      </c>
+      <c r="E13" s="16"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="13"/>
+      <c r="I13" s="13" t="s">
+        <v>206</v>
+      </c>
       <c r="J13" s="13"/>
-      <c r="K13" s="16" t="s">
+      <c r="K13" s="16"/>
+      <c r="L13" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="L13" s="13"/>
       <c r="M13" s="13"/>
       <c r="N13" s="33"/>
     </row>
@@ -9364,23 +9448,21 @@
       <c r="A14" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>205</v>
-      </c>
+      <c r="B14" s="16"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="16"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="16"/>
+      <c r="I14" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="I14" s="13"/>
       <c r="J14" s="13"/>
-      <c r="K14" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="L14" s="13"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="13" t="s">
+        <v>205</v>
+      </c>
       <c r="M14" s="13"/>
       <c r="N14" s="33"/>
     </row>
@@ -9388,21 +9470,21 @@
       <c r="A15" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>205</v>
-      </c>
+      <c r="B15" s="16"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="16"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
-      <c r="H15" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="I15" s="13"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="13" t="s">
+        <v>205</v>
+      </c>
       <c r="J15" s="13"/>
       <c r="K15" s="16"/>
-      <c r="L15" s="13"/>
+      <c r="L15" s="13" t="s">
+        <v>206</v>
+      </c>
       <c r="M15" s="13"/>
       <c r="N15" s="33"/>
     </row>
@@ -9415,19 +9497,15 @@
         <v>205</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="E16" s="16" t="s">
-        <v>205</v>
-      </c>
+      <c r="E16" s="16"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="16"/>
+      <c r="I16" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="I16" s="13"/>
       <c r="J16" s="13"/>
-      <c r="K16" s="16" t="s">
-        <v>205</v>
-      </c>
+      <c r="K16" s="16"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
       <c r="N16" s="33"/>
@@ -9441,24 +9519,22 @@
       <c r="D17" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>206</v>
-      </c>
+      <c r="E17" s="16"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="16"/>
+      <c r="I17" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="I17" s="13"/>
       <c r="J17" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="K17" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="L17" s="13"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="13" t="s">
+        <v>206</v>
+      </c>
       <c r="M17" s="13" t="s">
         <v>206</v>
       </c>
@@ -9472,17 +9548,17 @@
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
       <c r="E18" s="16"/>
-      <c r="F18" s="13" t="s">
-        <v>206</v>
-      </c>
+      <c r="F18" s="13"/>
       <c r="G18" s="13"/>
       <c r="H18" s="16"/>
-      <c r="I18" s="13"/>
+      <c r="I18" s="13" t="s">
+        <v>206</v>
+      </c>
       <c r="J18" s="13"/>
-      <c r="K18" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="L18" s="13"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="13" t="s">
+        <v>205</v>
+      </c>
       <c r="M18" s="13"/>
       <c r="N18" s="33"/>
     </row>
@@ -9490,27 +9566,23 @@
       <c r="A19" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>206</v>
-      </c>
+      <c r="B19" s="16"/>
       <c r="C19" s="13" t="s">
         <v>206</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="16"/>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="16" t="s">
+      <c r="J19" s="13"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="L19" s="13"/>
       <c r="M19" s="13"/>
       <c r="N19" s="33"/>
     </row>
@@ -9518,22 +9590,18 @@
       <c r="A20" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>205</v>
-      </c>
+      <c r="B20" s="16"/>
       <c r="C20" s="13" t="s">
         <v>205</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="16"/>
-      <c r="F20" s="13" t="s">
-        <v>206</v>
-      </c>
+      <c r="F20" s="13"/>
       <c r="G20" s="13"/>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="16"/>
+      <c r="I20" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="I20" s="13"/>
       <c r="J20" s="13"/>
       <c r="K20" s="16"/>
       <c r="L20" s="13" t="s">
@@ -9555,12 +9623,16 @@
       <c r="H21" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="I21" s="13"/>
+      <c r="I21" s="13" t="s">
+        <v>206</v>
+      </c>
       <c r="J21" s="13"/>
       <c r="K21" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="L21" s="13"/>
+      <c r="L21" s="13" t="s">
+        <v>206</v>
+      </c>
       <c r="M21" s="13"/>
       <c r="N21" s="33"/>
     </row>
@@ -9568,25 +9640,23 @@
       <c r="A22" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>206</v>
-      </c>
+      <c r="B22" s="16"/>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="16"/>
-      <c r="F22" s="13" t="s">
-        <v>205</v>
-      </c>
+      <c r="F22" s="13"/>
       <c r="G22" s="13"/>
       <c r="H22" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="I22" s="13"/>
+      <c r="I22" s="13" t="s">
+        <v>206</v>
+      </c>
       <c r="J22" s="13"/>
-      <c r="K22" s="16" t="s">
+      <c r="K22" s="16"/>
+      <c r="L22" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="L22" s="13"/>
       <c r="M22" s="13"/>
       <c r="N22" s="33"/>
     </row>
@@ -9598,12 +9668,12 @@
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
       <c r="E23" s="16"/>
-      <c r="F23" s="13" t="s">
-        <v>206</v>
-      </c>
+      <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="16"/>
-      <c r="I23" s="13"/>
+      <c r="I23" s="13" t="s">
+        <v>205</v>
+      </c>
       <c r="J23" s="13"/>
       <c r="K23" s="16"/>
       <c r="L23" s="13"/>
@@ -9620,19 +9690,21 @@
         <v>206</v>
       </c>
       <c r="E24" s="16"/>
-      <c r="F24" s="13" t="s">
-        <v>206</v>
-      </c>
+      <c r="F24" s="13"/>
       <c r="G24" s="13" t="s">
         <v>206</v>
       </c>
       <c r="H24" s="16"/>
-      <c r="I24" s="13"/>
+      <c r="I24" s="13" t="s">
+        <v>206</v>
+      </c>
       <c r="J24" s="13" t="s">
         <v>206</v>
       </c>
       <c r="K24" s="16"/>
-      <c r="L24" s="13"/>
+      <c r="L24" s="13" t="s">
+        <v>205</v>
+      </c>
       <c r="M24" s="13" t="s">
         <v>206</v>
       </c>
@@ -9642,21 +9714,21 @@
       <c r="A25" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>206</v>
-      </c>
+      <c r="B25" s="16"/>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
       <c r="E25" s="16"/>
-      <c r="F25" s="13" t="s">
-        <v>205</v>
-      </c>
+      <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="16"/>
-      <c r="I25" s="13"/>
+      <c r="I25" s="13" t="s">
+        <v>205</v>
+      </c>
       <c r="J25" s="13"/>
       <c r="K25" s="16"/>
-      <c r="L25" s="13"/>
+      <c r="L25" s="13" t="s">
+        <v>206</v>
+      </c>
       <c r="M25" s="13"/>
       <c r="N25" s="33"/>
     </row>
@@ -9681,7 +9753,7 @@
         <v>100</v>
       </c>
       <c r="B27" s="16">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C27" s="13">
         <v>5</v>
@@ -9690,28 +9762,28 @@
         <v>4</v>
       </c>
       <c r="E27" s="16">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F27" s="13">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G27" s="13">
         <v>4</v>
       </c>
       <c r="H27" s="16">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I27" s="13">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="J27" s="13">
         <v>4</v>
       </c>
       <c r="K27" s="16">
+        <v>3</v>
+      </c>
+      <c r="L27" s="13">
         <v>15</v>
-      </c>
-      <c r="L27" s="13">
-        <v>1</v>
       </c>
       <c r="M27" s="13">
         <v>4</v>
@@ -9732,31 +9804,31 @@
         <v>0.89</v>
       </c>
       <c r="E28" s="36">
+        <v>0.79</v>
+      </c>
+      <c r="F28" s="35">
+        <v>0.78</v>
+      </c>
+      <c r="G28" s="35">
+        <v>0.79</v>
+      </c>
+      <c r="H28" s="36">
+        <v>0.93</v>
+      </c>
+      <c r="I28" s="35">
+        <v>0.92</v>
+      </c>
+      <c r="J28" s="35">
+        <v>0.91</v>
+      </c>
+      <c r="K28" s="36">
+        <v>0.9</v>
+      </c>
+      <c r="L28" s="35">
         <v>0.88</v>
       </c>
-      <c r="F28" s="35">
-        <v>0.77</v>
-      </c>
-      <c r="G28" s="35">
-        <v>0.81</v>
-      </c>
-      <c r="H28" s="36">
-        <v>0.91</v>
-      </c>
-      <c r="I28" s="35">
-        <v>0.87</v>
-      </c>
-      <c r="J28" s="35">
-        <v>0.9</v>
-      </c>
-      <c r="K28" s="36">
-        <v>0.71</v>
-      </c>
-      <c r="L28" s="35">
-        <v>0.87</v>
-      </c>
       <c r="M28" s="35">
-        <v>0.79</v>
+        <v>0.82</v>
       </c>
       <c r="N28" s="33"/>
     </row>
@@ -9782,13 +9854,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="43"/>
+      <c r="A1" s="37"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>220</v>
       </c>
-      <c r="B2" s="44">
+      <c r="B2" s="38">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C2" t="s">
@@ -9820,10 +9892,10 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="B3" s="44">
+      <c r="B3" s="38">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C3" t="s">
@@ -9855,7 +9927,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="43"/>
+      <c r="A4" s="37"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -9869,27 +9941,27 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="45">
+      <c r="A6" s="39">
         <v>14.27206</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="40">
         <v>1</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="40">
         <v>1.5819559999999999E-4</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="43"/>
+      <c r="A7" s="37"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="43"/>
+      <c r="A8" s="37"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="B9" s="44">
+      <c r="B9" s="38">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C9" t="s">
@@ -9921,10 +9993,10 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="B10" s="44">
+      <c r="B10" s="38">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C10" t="s">
@@ -9956,7 +10028,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="43"/>
+      <c r="A11" s="37"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -9970,7 +10042,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="43">
+      <c r="A13" s="37">
         <v>8.2184162060000006</v>
       </c>
       <c r="B13">
@@ -9981,16 +10053,16 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="43"/>
+      <c r="A14" s="37"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="43"/>
+      <c r="A15" s="37"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="B16" s="44">
+      <c r="B16" s="38">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C16" t="s">
@@ -10022,10 +10094,10 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="B17" s="44">
+      <c r="B17" s="38">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C17" t="s">
@@ -10057,7 +10129,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="43"/>
+      <c r="A18" s="37"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -10071,24 +10143,24 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="45">
+      <c r="A20" s="39">
         <v>58.721420000000002</v>
       </c>
-      <c r="B20" s="46">
+      <c r="B20" s="40">
         <v>1</v>
       </c>
-      <c r="C20" s="46">
+      <c r="C20" s="40">
         <v>1.8207660000000001E-14</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="43"/>
+      <c r="A22" s="37"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>220</v>
       </c>
-      <c r="B23" s="44">
+      <c r="B23" s="38">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C23" t="s">
@@ -10120,10 +10192,10 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="B24" s="44">
+      <c r="B24" s="38">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C24" t="s">
@@ -10155,7 +10227,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="43"/>
+      <c r="A25" s="37"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -10169,171 +10241,171 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="45">
+      <c r="A27" s="39">
         <v>13.66929</v>
       </c>
-      <c r="B27" s="46">
+      <c r="B27" s="40">
         <v>1</v>
       </c>
-      <c r="C27" s="46">
+      <c r="C27" s="40">
         <v>2.179901E-4</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="43"/>
+      <c r="A28" s="37"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="43"/>
+      <c r="A29" s="37"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="43"/>
+      <c r="A30" s="37"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="43"/>
+      <c r="A31" s="37"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="43"/>
+      <c r="A32" s="37"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="43"/>
+      <c r="A33" s="37"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="43"/>
+      <c r="A34" s="37"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="43"/>
+      <c r="A35" s="37"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="43"/>
+      <c r="A36" s="37"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="43"/>
+      <c r="A37" s="37"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="43"/>
+      <c r="A38" s="37"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="43"/>
+      <c r="A39" s="37"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="43"/>
+      <c r="A40" s="37"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="43"/>
+      <c r="A41" s="37"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="43"/>
+      <c r="A43" s="37"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="43"/>
+      <c r="A45" s="37"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="43"/>
+      <c r="A46" s="37"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="43"/>
+      <c r="A47" s="37"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="43"/>
+      <c r="A48" s="37"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="43"/>
+      <c r="A49" s="37"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="43"/>
+      <c r="A50" s="37"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="43"/>
+      <c r="A51" s="37"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="43"/>
+      <c r="A52" s="37"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="43"/>
+      <c r="A53" s="37"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="43"/>
+      <c r="A54" s="37"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="43"/>
+      <c r="A55" s="37"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="43"/>
+      <c r="A56" s="37"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="43"/>
+      <c r="A57" s="37"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="43"/>
+      <c r="A58" s="37"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="43"/>
+      <c r="A59" s="37"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="43"/>
+      <c r="A60" s="37"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="43"/>
+      <c r="A61" s="37"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="43"/>
+      <c r="A62" s="37"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="43"/>
+      <c r="A64" s="37"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="43"/>
+      <c r="A66" s="37"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="43"/>
+      <c r="A67" s="37"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="43"/>
+      <c r="A68" s="37"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="43"/>
+      <c r="A69" s="37"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="43"/>
+      <c r="A70" s="37"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="43"/>
+      <c r="A71" s="37"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="43"/>
+      <c r="A72" s="37"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="43"/>
+      <c r="A73" s="37"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="43"/>
+      <c r="A74" s="37"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="43"/>
+      <c r="A75" s="37"/>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="43"/>
+      <c r="A76" s="37"/>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="43"/>
+      <c r="A77" s="37"/>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="43"/>
+      <c r="A78" s="37"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="43"/>
+      <c r="A79" s="37"/>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="43"/>
+      <c r="A80" s="37"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="43"/>
+      <c r="A81" s="37"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="43"/>
+      <c r="A82" s="37"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="43"/>
+      <c r="A83" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10342,15 +10414,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1880468A-055E-BA41-A377-B9D926328429}">
-  <dimension ref="A1:K87"/>
+  <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>225</v>
       </c>
@@ -10364,7 +10436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>228</v>
       </c>
@@ -10396,7 +10468,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>40</v>
       </c>
@@ -10409,20 +10481,20 @@
       <c r="E4">
         <v>31.838999999999999</v>
       </c>
-      <c r="F4">
-        <v>2.6297000000000001</v>
+      <c r="F4" s="40">
+        <v>11.329000000000001</v>
       </c>
       <c r="G4">
-        <v>0.28992000000000001</v>
-      </c>
-      <c r="H4">
-        <v>2.0615000000000001</v>
-      </c>
-      <c r="I4">
-        <v>3.1979000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>5.9211</v>
+      </c>
+      <c r="H4" s="40">
+        <v>-0.27594000000000002</v>
+      </c>
+      <c r="I4" s="40">
+        <v>22.934000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>236</v>
       </c>
@@ -10438,20 +10510,20 @@
       <c r="F5">
         <v>31.838999999999999</v>
       </c>
-      <c r="G5">
-        <v>13.87</v>
+      <c r="G5" s="40">
+        <v>83215</v>
       </c>
       <c r="H5" t="s">
         <v>238</v>
       </c>
-      <c r="I5">
-        <v>7.8574000000000002</v>
-      </c>
-      <c r="J5">
-        <v>24.481999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I5" s="40">
+        <v>0.75885999999999998</v>
+      </c>
+      <c r="J5" s="40">
+        <v>9125200000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>42</v>
       </c>
@@ -10464,20 +10536,20 @@
       <c r="E6">
         <v>19.53</v>
       </c>
-      <c r="F6">
-        <v>1.6278999999999999</v>
+      <c r="F6" s="40">
+        <v>-3.7461000000000002</v>
       </c>
       <c r="G6">
-        <v>0.30807000000000001</v>
-      </c>
-      <c r="H6">
-        <v>1.0241</v>
-      </c>
-      <c r="I6">
-        <v>2.2317</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.5760999999999998</v>
+      </c>
+      <c r="H6" s="40">
+        <v>-10.755000000000001</v>
+      </c>
+      <c r="I6" s="40">
+        <v>3.2629000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>236</v>
       </c>
@@ -10493,20 +10565,20 @@
       <c r="F7">
         <v>19.53</v>
       </c>
-      <c r="G7">
-        <v>5.0932000000000004</v>
+      <c r="G7" s="40">
+        <v>2.3609000000000002E-2</v>
       </c>
       <c r="H7" t="s">
         <v>238</v>
       </c>
-      <c r="I7">
-        <v>2.7846000000000002</v>
-      </c>
-      <c r="J7">
-        <v>9.3157999999999994</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I7" s="40">
+        <v>2.1335000000000002E-5</v>
+      </c>
+      <c r="J7" s="40">
+        <v>26.126000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>51</v>
       </c>
@@ -10519,20 +10591,20 @@
       <c r="E8">
         <v>16.667000000000002</v>
       </c>
-      <c r="F8">
-        <v>0.20895</v>
+      <c r="F8" s="40">
+        <v>0.22297</v>
       </c>
       <c r="G8">
-        <v>0.13783000000000001</v>
-      </c>
-      <c r="H8">
-        <v>-6.1192000000000003E-2</v>
-      </c>
-      <c r="I8">
-        <v>0.47910000000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.14026</v>
+      </c>
+      <c r="H8" s="40">
+        <v>-5.1929999999999997E-2</v>
+      </c>
+      <c r="I8" s="40">
+        <v>0.49787999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>236</v>
       </c>
@@ -10548,46 +10620,46 @@
       <c r="F9">
         <v>16.667000000000002</v>
       </c>
-      <c r="G9">
-        <v>1.2323999999999999</v>
+      <c r="G9" s="40">
+        <v>1.2498</v>
       </c>
       <c r="H9" t="s">
         <v>238</v>
       </c>
-      <c r="I9">
-        <v>0.94064000000000003</v>
-      </c>
-      <c r="J9">
-        <v>1.6146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I9" s="40">
+        <v>0.94938999999999996</v>
+      </c>
+      <c r="J9" s="40">
+        <v>1.6452</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C10">
-        <v>7.1333000000000002</v>
+        <v>7</v>
       </c>
       <c r="D10">
-        <v>8.7667000000000002</v>
+        <v>21</v>
       </c>
       <c r="E10">
-        <v>1.6333</v>
-      </c>
-      <c r="F10">
-        <v>0.41367999999999999</v>
+        <v>14</v>
+      </c>
+      <c r="F10" s="40">
+        <v>-3.0402999999999998</v>
       </c>
       <c r="G10">
-        <v>0.12343999999999999</v>
-      </c>
-      <c r="H10">
-        <v>0.17174</v>
-      </c>
-      <c r="I10">
-        <v>0.65563000000000005</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>2.6067</v>
+      </c>
+      <c r="H10" s="40">
+        <v>-8.1493000000000002</v>
+      </c>
+      <c r="I10" s="40">
+        <v>2.0688</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>236</v>
       </c>
@@ -10595,42 +10667,83 @@
         <v>237</v>
       </c>
       <c r="D11">
-        <v>7.1333000000000002</v>
+        <v>7</v>
       </c>
       <c r="E11">
-        <v>8.7667000000000002</v>
+        <v>21</v>
       </c>
       <c r="F11">
-        <v>1.6333</v>
-      </c>
-      <c r="G11">
-        <v>1.5124</v>
+        <v>14</v>
+      </c>
+      <c r="G11" s="40">
+        <v>4.7822000000000003E-2</v>
       </c>
       <c r="H11" t="s">
         <v>238</v>
       </c>
-      <c r="I11">
-        <v>1.1874</v>
-      </c>
-      <c r="J11">
-        <v>1.9263999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>239</v>
-      </c>
+      <c r="I11" s="40">
+        <v>2.8892000000000002E-4</v>
+      </c>
+      <c r="J11" s="40">
+        <v>7.9154</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12">
+        <v>7.1333000000000002</v>
+      </c>
+      <c r="D12">
+        <v>8.7667000000000002</v>
+      </c>
+      <c r="E12">
+        <v>1.6333</v>
+      </c>
+      <c r="F12" s="40">
+        <v>0.48903000000000002</v>
+      </c>
+      <c r="G12">
+        <v>0.23946000000000001</v>
+      </c>
+      <c r="H12" s="40">
+        <v>1.9701E-2</v>
+      </c>
+      <c r="I12" s="40">
+        <v>0.95835999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C13" t="s">
-        <v>241</v>
-      </c>
-      <c r="D13" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+      <c r="D13">
+        <v>7.1333000000000002</v>
+      </c>
+      <c r="E13">
+        <v>8.7667000000000002</v>
+      </c>
+      <c r="F13">
+        <v>1.6333</v>
+      </c>
+      <c r="G13" s="40">
+        <v>1.6307</v>
+      </c>
+      <c r="H13" t="s">
+        <v>238</v>
+      </c>
+      <c r="I13" s="40">
+        <v>1.0199</v>
+      </c>
+      <c r="J13" s="40">
+        <v>2.6074000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>225</v>
       </c>
@@ -10644,7 +10757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>228</v>
       </c>
@@ -10676,7 +10789,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>40</v>
       </c>
@@ -10689,20 +10802,20 @@
       <c r="E18">
         <v>31.838999999999999</v>
       </c>
-      <c r="F18">
-        <v>1.5619000000000001</v>
+      <c r="F18" s="40">
+        <v>13.866</v>
       </c>
       <c r="G18">
-        <v>0.40821000000000002</v>
-      </c>
-      <c r="H18">
-        <v>0.76185000000000003</v>
-      </c>
-      <c r="I18">
-        <v>2.3620000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+        <v>6.9396000000000004</v>
+      </c>
+      <c r="H18" s="40">
+        <v>0.26488</v>
+      </c>
+      <c r="I18" s="40">
+        <v>27.466999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>236</v>
       </c>
@@ -10718,20 +10831,20 @@
       <c r="F19">
         <v>31.838999999999999</v>
       </c>
-      <c r="G19">
-        <v>4.7679999999999998</v>
+      <c r="G19" s="40">
+        <v>1052000</v>
       </c>
       <c r="H19" t="s">
         <v>238</v>
       </c>
-      <c r="I19">
-        <v>2.1421999999999999</v>
-      </c>
-      <c r="J19">
-        <v>10.612</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I19" s="40">
+        <v>1.3032999999999999</v>
+      </c>
+      <c r="J19" s="40">
+        <v>849130000000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>42</v>
       </c>
@@ -10744,20 +10857,20 @@
       <c r="E20">
         <v>19.53</v>
       </c>
-      <c r="F20">
-        <v>1.7090000000000001</v>
+      <c r="F20" s="40">
+        <v>-4.5547000000000004</v>
       </c>
       <c r="G20">
-        <v>0.43181999999999998</v>
-      </c>
-      <c r="H20">
-        <v>0.86265000000000003</v>
-      </c>
-      <c r="I20">
-        <v>2.5552999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+        <v>4.1223999999999998</v>
+      </c>
+      <c r="H20" s="40">
+        <v>-12.634</v>
+      </c>
+      <c r="I20" s="40">
+        <v>3.5249999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>236</v>
       </c>
@@ -10773,46 +10886,46 @@
       <c r="F21">
         <v>19.53</v>
       </c>
-      <c r="G21">
-        <v>5.5233999999999996</v>
+      <c r="G21" s="40">
+        <v>1.0518E-2</v>
       </c>
       <c r="H21" t="s">
         <v>238</v>
       </c>
-      <c r="I21">
-        <v>2.3694000000000002</v>
-      </c>
-      <c r="J21">
-        <v>12.875999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I21" s="40">
+        <v>3.258E-6</v>
+      </c>
+      <c r="J21" s="40">
+        <v>33.954000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C22">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="D22">
-        <v>126.67</v>
+        <v>21</v>
       </c>
       <c r="E22">
-        <v>16.667000000000002</v>
-      </c>
-      <c r="F22">
-        <v>0.15339</v>
+        <v>14</v>
+      </c>
+      <c r="F22" s="40">
+        <v>-2.5173999999999999</v>
       </c>
       <c r="G22">
-        <v>0.21007999999999999</v>
-      </c>
-      <c r="H22">
-        <v>-0.25836999999999999</v>
-      </c>
-      <c r="I22">
-        <v>0.56513999999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.0882000000000001</v>
+      </c>
+      <c r="H22" s="40">
+        <v>-8.5701999999999998</v>
+      </c>
+      <c r="I22" s="40">
+        <v>3.5352999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>236</v>
       </c>
@@ -10820,54 +10933,54 @@
         <v>237</v>
       </c>
       <c r="D23">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="E23">
-        <v>126.67</v>
+        <v>21</v>
       </c>
       <c r="F23">
-        <v>16.667000000000002</v>
-      </c>
-      <c r="G23">
-        <v>1.1657999999999999</v>
+        <v>14</v>
+      </c>
+      <c r="G23" s="40">
+        <v>8.0667000000000003E-2</v>
       </c>
       <c r="H23" t="s">
         <v>238</v>
       </c>
-      <c r="I23">
-        <v>0.77231000000000005</v>
-      </c>
-      <c r="J23">
-        <v>1.7597</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I23" s="40">
+        <v>1.8966999999999999E-4</v>
+      </c>
+      <c r="J23" s="40">
+        <v>34.307000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C24">
-        <v>7.1333000000000002</v>
+        <v>110</v>
       </c>
       <c r="D24">
-        <v>8.7667000000000002</v>
+        <v>126.67</v>
       </c>
       <c r="E24">
-        <v>1.6333</v>
-      </c>
-      <c r="F24">
-        <v>0.30254999999999999</v>
+        <v>16.667000000000002</v>
+      </c>
+      <c r="F24" s="40">
+        <v>0.19153999999999999</v>
       </c>
       <c r="G24">
-        <v>0.17274</v>
-      </c>
-      <c r="H24">
-        <v>-3.6006000000000003E-2</v>
-      </c>
-      <c r="I24">
-        <v>0.64110999999999996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.21576000000000001</v>
+      </c>
+      <c r="H24" s="40">
+        <v>-0.23133999999999999</v>
+      </c>
+      <c r="I24" s="40">
+        <v>0.61441999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>236</v>
       </c>
@@ -10875,42 +10988,83 @@
         <v>237</v>
       </c>
       <c r="D25">
-        <v>7.1333000000000002</v>
+        <v>110</v>
       </c>
       <c r="E25">
-        <v>8.7667000000000002</v>
+        <v>126.67</v>
       </c>
       <c r="F25">
-        <v>1.6333</v>
-      </c>
-      <c r="G25">
-        <v>1.3532999999999999</v>
+        <v>16.667000000000002</v>
+      </c>
+      <c r="G25" s="40">
+        <v>1.2111000000000001</v>
       </c>
       <c r="H25" t="s">
         <v>238</v>
       </c>
-      <c r="I25">
-        <v>0.96462999999999999</v>
-      </c>
-      <c r="J25">
-        <v>1.8986000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>239</v>
-      </c>
+      <c r="I25" s="40">
+        <v>0.79347000000000001</v>
+      </c>
+      <c r="J25" s="40">
+        <v>1.8486</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26">
+        <v>7.1333000000000002</v>
+      </c>
+      <c r="D26">
+        <v>8.7667000000000002</v>
+      </c>
+      <c r="E26">
+        <v>1.6333</v>
+      </c>
+      <c r="F26" s="40">
+        <v>0.25953999999999999</v>
+      </c>
+      <c r="G26">
+        <v>0.36853999999999998</v>
+      </c>
+      <c r="H26" s="40">
+        <v>-0.46278999999999998</v>
+      </c>
+      <c r="I26" s="40">
+        <v>0.98187000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C27" t="s">
-        <v>241</v>
-      </c>
-      <c r="D27" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+      <c r="D27">
+        <v>7.1333000000000002</v>
+      </c>
+      <c r="E27">
+        <v>8.7667000000000002</v>
+      </c>
+      <c r="F27">
+        <v>1.6333</v>
+      </c>
+      <c r="G27" s="40">
+        <v>1.2963</v>
+      </c>
+      <c r="H27" t="s">
+        <v>238</v>
+      </c>
+      <c r="I27" s="40">
+        <v>0.62953000000000003</v>
+      </c>
+      <c r="J27" s="40">
+        <v>2.6694</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>225</v>
       </c>
@@ -10924,7 +11078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>228</v>
       </c>
@@ -10956,7 +11110,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>40</v>
       </c>
@@ -10970,19 +11124,19 @@
         <v>31.838999999999999</v>
       </c>
       <c r="F32">
-        <v>1.6291</v>
+        <v>4.2435</v>
       </c>
       <c r="G32">
-        <v>0.32346999999999998</v>
+        <v>6.0075000000000003</v>
       </c>
       <c r="H32">
-        <v>0.99506000000000006</v>
-      </c>
-      <c r="I32">
-        <v>2.2631000000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+        <v>-7.5311000000000003</v>
+      </c>
+      <c r="I32" s="40">
+        <v>16.018000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>236</v>
       </c>
@@ -10999,19 +11153,19 @@
         <v>31.838999999999999</v>
       </c>
       <c r="G33">
-        <v>5.0991</v>
+        <v>69.650999999999996</v>
       </c>
       <c r="H33" t="s">
         <v>238</v>
       </c>
       <c r="I33">
-        <v>2.7048999999999999</v>
-      </c>
-      <c r="J33">
-        <v>9.6123999999999992</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+        <v>5.3616999999999998E-4</v>
+      </c>
+      <c r="J33" s="40">
+        <v>9047900</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>42</v>
       </c>
@@ -11025,19 +11179,19 @@
         <v>19.53</v>
       </c>
       <c r="F34">
-        <v>3.8178000000000001</v>
+        <v>4.0008999999999997</v>
       </c>
       <c r="G34">
-        <v>0.35504999999999998</v>
+        <v>3.7159</v>
       </c>
       <c r="H34">
-        <v>3.1219000000000001</v>
-      </c>
-      <c r="I34">
-        <v>4.5137</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+        <v>-3.2820999999999998</v>
+      </c>
+      <c r="I34" s="40">
+        <v>11.284000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>236</v>
       </c>
@@ -11054,45 +11208,45 @@
         <v>19.53</v>
       </c>
       <c r="G35">
-        <v>45.503999999999998</v>
+        <v>54.645000000000003</v>
       </c>
       <c r="H35" t="s">
         <v>238</v>
       </c>
       <c r="I35">
-        <v>22.69</v>
-      </c>
-      <c r="J35">
-        <v>91.257999999999996</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.7547999999999998E-2</v>
+      </c>
+      <c r="J35" s="40">
+        <v>79526</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C36">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="D36">
-        <v>126.67</v>
+        <v>21</v>
       </c>
       <c r="E36">
-        <v>16.667000000000002</v>
+        <v>14</v>
       </c>
       <c r="F36">
-        <v>0.53066999999999998</v>
+        <v>-0.67383000000000004</v>
       </c>
       <c r="G36">
-        <v>0.14199000000000001</v>
+        <v>2.6373000000000002</v>
       </c>
       <c r="H36">
-        <v>0.25237999999999999</v>
-      </c>
-      <c r="I36">
-        <v>0.80896000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+        <v>-5.8428000000000004</v>
+      </c>
+      <c r="I36" s="40">
+        <v>4.4951999999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>236</v>
       </c>
@@ -11100,54 +11254,54 @@
         <v>237</v>
       </c>
       <c r="D37">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="E37">
-        <v>126.67</v>
+        <v>21</v>
       </c>
       <c r="F37">
-        <v>16.667000000000002</v>
+        <v>14</v>
       </c>
       <c r="G37">
-        <v>1.7000999999999999</v>
+        <v>0.50975000000000004</v>
       </c>
       <c r="H37" t="s">
         <v>238</v>
       </c>
       <c r="I37">
-        <v>1.2870999999999999</v>
-      </c>
-      <c r="J37">
-        <v>2.2456</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+        <v>2.9006000000000001E-3</v>
+      </c>
+      <c r="J37" s="40">
+        <v>89.584999999999994</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C38">
-        <v>7.1333000000000002</v>
+        <v>110</v>
       </c>
       <c r="D38">
-        <v>8.7667000000000002</v>
+        <v>126.67</v>
       </c>
       <c r="E38">
-        <v>1.6333</v>
+        <v>16.667000000000002</v>
       </c>
       <c r="F38">
-        <v>0.21965999999999999</v>
+        <v>0.55112000000000005</v>
       </c>
       <c r="G38">
-        <v>0.12554000000000001</v>
+        <v>0.14482999999999999</v>
       </c>
       <c r="H38">
-        <v>-2.6404E-2</v>
-      </c>
-      <c r="I38">
-        <v>0.46571000000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.26727000000000001</v>
+      </c>
+      <c r="I38" s="40">
+        <v>0.83496999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>236</v>
       </c>
@@ -11155,42 +11309,83 @@
         <v>237</v>
       </c>
       <c r="D39">
-        <v>7.1333000000000002</v>
+        <v>110</v>
       </c>
       <c r="E39">
-        <v>8.7667000000000002</v>
+        <v>126.67</v>
       </c>
       <c r="F39">
-        <v>1.6333</v>
+        <v>16.667000000000002</v>
       </c>
       <c r="G39">
-        <v>1.2456</v>
+        <v>1.7352000000000001</v>
       </c>
       <c r="H39" t="s">
         <v>238</v>
       </c>
       <c r="I39">
-        <v>0.97394000000000003</v>
-      </c>
-      <c r="J39">
-        <v>1.5931999999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>239</v>
-      </c>
+        <v>1.3064</v>
+      </c>
+      <c r="J39" s="40">
+        <v>2.3048000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40">
+        <v>7.1333000000000002</v>
+      </c>
+      <c r="D40">
+        <v>8.7667000000000002</v>
+      </c>
+      <c r="E40">
+        <v>1.6333</v>
+      </c>
+      <c r="F40">
+        <v>0.21193999999999999</v>
+      </c>
+      <c r="G40">
+        <v>0.24096000000000001</v>
+      </c>
+      <c r="H40">
+        <v>-0.26033000000000001</v>
+      </c>
+      <c r="I40" s="40">
+        <v>0.68420999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C41" t="s">
-        <v>241</v>
-      </c>
-      <c r="D41" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+      <c r="D41">
+        <v>7.1333000000000002</v>
+      </c>
+      <c r="E41">
+        <v>8.7667000000000002</v>
+      </c>
+      <c r="F41">
+        <v>1.6333</v>
+      </c>
+      <c r="G41">
+        <v>1.2361</v>
+      </c>
+      <c r="H41" t="s">
+        <v>238</v>
+      </c>
+      <c r="I41">
+        <v>0.77080000000000004</v>
+      </c>
+      <c r="J41" s="40">
+        <v>1.9822</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>225</v>
       </c>
@@ -11204,7 +11399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>228</v>
       </c>
@@ -11236,7 +11431,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>40</v>
       </c>
@@ -11249,20 +11444,20 @@
       <c r="E46">
         <v>31.838999999999999</v>
       </c>
-      <c r="F46">
-        <v>1.0181</v>
+      <c r="F46" s="40">
+        <v>18.189</v>
       </c>
       <c r="G46">
-        <v>0.37353999999999998</v>
-      </c>
-      <c r="H46">
-        <v>0.28597</v>
-      </c>
-      <c r="I46">
-        <v>1.7502</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+        <v>7.9683000000000002</v>
+      </c>
+      <c r="H46" s="40">
+        <v>2.5718000000000001</v>
+      </c>
+      <c r="I46" s="40">
+        <v>33.807000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>236</v>
       </c>
@@ -11278,20 +11473,20 @@
       <c r="F47">
         <v>31.838999999999999</v>
       </c>
-      <c r="G47">
-        <v>2.7679</v>
+      <c r="G47" s="40">
+        <v>79349000</v>
       </c>
       <c r="H47" t="s">
         <v>238</v>
       </c>
-      <c r="I47">
-        <v>1.331</v>
-      </c>
-      <c r="J47">
-        <v>5.7557999999999998</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I47" s="40">
+        <v>13.09</v>
+      </c>
+      <c r="J47" s="40">
+        <v>481010000000000</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>42</v>
       </c>
@@ -11304,17 +11499,17 @@
       <c r="E48">
         <v>19.53</v>
       </c>
-      <c r="F48">
-        <v>2.0695999999999999</v>
+      <c r="F48" s="40">
+        <v>-8.6631</v>
       </c>
       <c r="G48">
-        <v>0.37592999999999999</v>
-      </c>
-      <c r="H48">
-        <v>1.3328</v>
-      </c>
-      <c r="I48">
-        <v>2.8064</v>
+        <v>4.8284000000000002</v>
+      </c>
+      <c r="H48" s="40">
+        <v>-18.126999999999999</v>
+      </c>
+      <c r="I48" s="40">
+        <v>0.80035000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
@@ -11333,43 +11528,43 @@
       <c r="F49">
         <v>19.53</v>
       </c>
-      <c r="G49">
-        <v>7.9215</v>
+      <c r="G49" s="40">
+        <v>1.7284000000000001E-4</v>
       </c>
       <c r="H49" t="s">
         <v>238</v>
       </c>
-      <c r="I49">
-        <v>3.7915000000000001</v>
-      </c>
-      <c r="J49">
-        <v>16.55</v>
+      <c r="I49" s="40">
+        <v>1.3418999999999999E-8</v>
+      </c>
+      <c r="J49" s="40">
+        <v>2.2263000000000002</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C50">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="D50">
-        <v>126.67</v>
+        <v>21</v>
       </c>
       <c r="E50">
-        <v>16.667000000000002</v>
-      </c>
-      <c r="F50">
-        <v>0.58069999999999999</v>
+        <v>14</v>
+      </c>
+      <c r="F50" s="40">
+        <v>-6.8796999999999997</v>
       </c>
       <c r="G50">
-        <v>0.18149999999999999</v>
-      </c>
-      <c r="H50">
-        <v>0.22495999999999999</v>
-      </c>
-      <c r="I50">
-        <v>0.93644000000000005</v>
+        <v>3.5139999999999998</v>
+      </c>
+      <c r="H50" s="40">
+        <v>-13.766999999999999</v>
+      </c>
+      <c r="I50" s="40">
+        <v>7.6572999999999997E-3</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -11380,51 +11575,51 @@
         <v>237</v>
       </c>
       <c r="D51">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="E51">
-        <v>126.67</v>
+        <v>21</v>
       </c>
       <c r="F51">
-        <v>16.667000000000002</v>
-      </c>
-      <c r="G51">
-        <v>1.7873000000000001</v>
+        <v>14</v>
+      </c>
+      <c r="G51" s="40">
+        <v>1.0284000000000001E-3</v>
       </c>
       <c r="H51" t="s">
         <v>238</v>
       </c>
-      <c r="I51">
-        <v>1.2523</v>
-      </c>
-      <c r="J51">
-        <v>2.5508999999999999</v>
+      <c r="I51" s="40">
+        <v>1.0496000000000001E-6</v>
+      </c>
+      <c r="J51" s="40">
+        <v>1.0077</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C52">
-        <v>7.1333000000000002</v>
+        <v>110</v>
       </c>
       <c r="D52">
-        <v>8.7667000000000002</v>
+        <v>126.67</v>
       </c>
       <c r="E52">
-        <v>1.6333</v>
-      </c>
-      <c r="F52">
-        <v>0.44595000000000001</v>
+        <v>16.667000000000002</v>
+      </c>
+      <c r="F52" s="40">
+        <v>0.57843</v>
       </c>
       <c r="G52">
-        <v>0.15054999999999999</v>
-      </c>
-      <c r="H52">
-        <v>0.15087</v>
-      </c>
-      <c r="I52">
-        <v>0.74102000000000001</v>
+        <v>0.18620999999999999</v>
+      </c>
+      <c r="H52" s="40">
+        <v>0.21346000000000001</v>
+      </c>
+      <c r="I52" s="40">
+        <v>0.94340000000000002</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -11435,359 +11630,1458 @@
         <v>237</v>
       </c>
       <c r="D53">
-        <v>7.1333000000000002</v>
+        <v>110</v>
       </c>
       <c r="E53">
-        <v>8.7667000000000002</v>
+        <v>126.67</v>
       </c>
       <c r="F53">
-        <v>1.6333</v>
-      </c>
-      <c r="G53">
-        <v>1.5620000000000001</v>
+        <v>16.667000000000002</v>
+      </c>
+      <c r="G53" s="40">
+        <v>1.7831999999999999</v>
       </c>
       <c r="H53" t="s">
         <v>238</v>
       </c>
-      <c r="I53">
-        <v>1.1628000000000001</v>
-      </c>
-      <c r="J53">
-        <v>2.0981000000000001</v>
+      <c r="I53" s="40">
+        <v>1.238</v>
+      </c>
+      <c r="J53" s="40">
+        <v>2.5687000000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54">
+        <v>7.1333000000000002</v>
+      </c>
+      <c r="D54">
+        <v>8.7667000000000002</v>
+      </c>
+      <c r="E54">
+        <v>1.6333</v>
+      </c>
+      <c r="F54" s="40">
+        <v>0.39133000000000001</v>
+      </c>
+      <c r="G54">
+        <v>0.31381999999999999</v>
+      </c>
+      <c r="H54" s="40">
+        <v>-0.22375</v>
+      </c>
+      <c r="I54" s="40">
+        <v>1.0064</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="B55" t="s">
+        <v>236</v>
+      </c>
+      <c r="C55" t="s">
+        <v>237</v>
+      </c>
+      <c r="D55">
+        <v>7.1333000000000002</v>
+      </c>
+      <c r="E55">
+        <v>8.7667000000000002</v>
+      </c>
+      <c r="F55">
+        <v>1.6333</v>
+      </c>
+      <c r="G55" s="40">
+        <v>1.4789000000000001</v>
+      </c>
+      <c r="H55" t="s">
+        <v>238</v>
+      </c>
+      <c r="I55" s="40">
+        <v>0.79951000000000005</v>
+      </c>
+      <c r="J55" s="40">
+        <v>2.7357999999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>263</v>
+      </c>
+      <c r="H60" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>264</v>
+      </c>
+      <c r="H61" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H62" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H63" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>265</v>
+      </c>
+      <c r="H64" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H65" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>266</v>
+      </c>
+      <c r="H66" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>267</v>
+      </c>
+      <c r="H67" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H69" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>268</v>
+      </c>
+      <c r="H70" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H73" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>270</v>
+      </c>
+      <c r="H74" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>271</v>
+      </c>
+      <c r="H75" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H76" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H77" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H78" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H79" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H80" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="82" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H82" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="83" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H83" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="86" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H86" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="87" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H87" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="88" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H88" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="89" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H89" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="90" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H90" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="91" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H91" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="92" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H92" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="93" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H93" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="95" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H95" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="96" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H96" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="99" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H99" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="100" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H100" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="101" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H101" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="102" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H102" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="103" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H103" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="104" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H104" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="105" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H105" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="106" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H106" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="108" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H108" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="109" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H109" t="s">
+        <v>296</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2987885-C709-614F-8DFD-D0F729A65828}">
+  <dimension ref="A1:I50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
         <v>239</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C1" t="s">
         <v>240</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D1" t="s">
         <v>241</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="F1" t="s">
         <v>243</v>
       </c>
-      <c r="B58" t="s">
-        <v>36</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="G1" t="s">
         <v>244</v>
       </c>
-      <c r="D58" t="s">
+      <c r="H1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>245</v>
       </c>
-      <c r="E58" t="s">
-        <v>36</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="B2">
+        <v>0.76380000000000003</v>
+      </c>
+      <c r="C2">
+        <v>0.77429999999999999</v>
+      </c>
+      <c r="D2">
+        <v>0.75739999999999996</v>
+      </c>
+      <c r="E2">
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="F2">
+        <v>0.74690000000000001</v>
+      </c>
+      <c r="G2">
+        <v>500</v>
+      </c>
+      <c r="H2">
+        <f>0.5*(F2+1)</f>
+        <v>0.87345000000000006</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>246</v>
       </c>
-      <c r="G58" t="s">
+      <c r="B3">
+        <v>0.4103</v>
+      </c>
+      <c r="C3">
+        <v>0.42370000000000002</v>
+      </c>
+      <c r="D3">
+        <v>0.39810000000000001</v>
+      </c>
+      <c r="E3">
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="F3">
+        <v>0.38469999999999999</v>
+      </c>
+      <c r="G3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>0.9</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>-8.3500000000000005E-2</v>
+      </c>
+      <c r="E4">
+        <v>8.3500000000000005E-2</v>
+      </c>
+      <c r="F4">
+        <v>-8.3500000000000005E-2</v>
+      </c>
+      <c r="G4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>248</v>
       </c>
-      <c r="C59" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0.9123</v>
+      </c>
+      <c r="E5">
+        <v>8.77E-2</v>
+      </c>
+      <c r="F5">
+        <v>0.9123</v>
+      </c>
+      <c r="G5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>249</v>
       </c>
-      <c r="D59" t="s">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>3.5299999999999998E-2</v>
+      </c>
+      <c r="E6">
+        <v>3.5299999999999998E-2</v>
+      </c>
+      <c r="F6">
+        <v>3.5299999999999998E-2</v>
+      </c>
+      <c r="G6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B7">
+        <v>0.247</v>
+      </c>
+      <c r="C7">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="D7">
+        <v>0.2387</v>
+      </c>
+      <c r="E7">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.2298</v>
+      </c>
+      <c r="G7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B8">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="C8">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="D8">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="E8">
+        <v>-2.7000000000000001E-3</v>
+      </c>
+      <c r="F8">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="G8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B9">
+        <v>0.2485</v>
+      </c>
+      <c r="C9">
+        <v>0.25750000000000001</v>
+      </c>
+      <c r="D9">
+        <v>0.23760000000000001</v>
+      </c>
+      <c r="E9">
+        <v>1.9900000000000001E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.2286</v>
+      </c>
+      <c r="G9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B10">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="C10">
+        <v>8.1100000000000005E-2</v>
+      </c>
+      <c r="D10">
+        <v>8.4699999999999998E-2</v>
+      </c>
+      <c r="E10">
+        <v>-3.5999999999999999E-3</v>
+      </c>
+      <c r="F10">
+        <v>8.6900000000000005E-2</v>
+      </c>
+      <c r="G10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>254</v>
+      </c>
+      <c r="B11">
+        <v>2.9933000000000001</v>
+      </c>
+      <c r="C11">
+        <v>3.1646999999999998</v>
+      </c>
+      <c r="D11">
+        <v>2.8689</v>
+      </c>
+      <c r="E11">
+        <v>0.29580000000000001</v>
+      </c>
+      <c r="F11">
+        <v>2.6974999999999998</v>
+      </c>
+      <c r="G11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>255</v>
+      </c>
+      <c r="B12">
+        <v>0.17119999999999999</v>
+      </c>
+      <c r="C12">
+        <v>0.17280000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.16880000000000001</v>
+      </c>
+      <c r="E12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F12">
+        <v>0.16719999999999999</v>
+      </c>
+      <c r="G12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C14" t="s">
+        <v>258</v>
+      </c>
+      <c r="D14" t="s">
+        <v>259</v>
+      </c>
+      <c r="E14">
+        <v>31</v>
+      </c>
+      <c r="F14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C15" t="s">
+        <v>240</v>
+      </c>
+      <c r="D15" t="s">
+        <v>241</v>
+      </c>
+      <c r="E15" t="s">
+        <v>242</v>
+      </c>
+      <c r="F15" t="s">
+        <v>243</v>
+      </c>
+      <c r="G15" t="s">
         <v>244</v>
       </c>
-      <c r="E59" t="s">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>245</v>
+      </c>
+      <c r="B16">
+        <v>0.7661</v>
+      </c>
+      <c r="C16">
+        <v>0.7843</v>
+      </c>
+      <c r="D16">
+        <v>0.74429999999999996</v>
+      </c>
+      <c r="E16">
+        <v>0.04</v>
+      </c>
+      <c r="F16">
+        <v>0.72609999999999997</v>
+      </c>
+      <c r="G16">
+        <v>469</v>
+      </c>
+      <c r="H16">
+        <f>0.5*(F16+1)</f>
+        <v>0.86304999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>246</v>
+      </c>
+      <c r="B17">
+        <v>0.28789999999999999</v>
+      </c>
+      <c r="C17">
+        <v>0.3155</v>
+      </c>
+      <c r="D17">
+        <v>0.26329999999999998</v>
+      </c>
+      <c r="E17">
+        <v>5.21E-2</v>
+      </c>
+      <c r="F17">
+        <v>0.23569999999999999</v>
+      </c>
+      <c r="G17">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>247</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>-0.51690000000000003</v>
+      </c>
+      <c r="E18">
+        <v>0.51690000000000003</v>
+      </c>
+      <c r="F18">
+        <v>-0.51690000000000003</v>
+      </c>
+      <c r="G18">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>248</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0.75490000000000002</v>
+      </c>
+      <c r="E19">
+        <v>0.24510000000000001</v>
+      </c>
+      <c r="F19">
+        <v>0.75490000000000002</v>
+      </c>
+      <c r="G19">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>249</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0.1726</v>
+      </c>
+      <c r="E20">
+        <v>0.1726</v>
+      </c>
+      <c r="F20">
+        <v>0.1726</v>
+      </c>
+      <c r="G20">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="B21">
+        <v>8.5699999999999998E-2</v>
+      </c>
+      <c r="C21">
+        <v>9.4100000000000003E-2</v>
+      </c>
+      <c r="D21">
+        <v>7.8E-2</v>
+      </c>
+      <c r="E21">
+        <v>1.61E-2</v>
+      </c>
+      <c r="F21">
+        <v>6.9699999999999998E-2</v>
+      </c>
+      <c r="G21">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>251</v>
       </c>
-      <c r="B62" t="s">
-        <v>36</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="B22">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="C22">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="D22">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E22">
+        <v>-5.4999999999999997E-3</v>
+      </c>
+      <c r="F22">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G22">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>252</v>
+      </c>
+      <c r="B23">
+        <v>8.72E-2</v>
+      </c>
+      <c r="C23">
+        <v>9.5600000000000004E-2</v>
+      </c>
+      <c r="D23">
+        <v>7.4099999999999999E-2</v>
+      </c>
+      <c r="E23">
+        <v>2.1499999999999998E-2</v>
+      </c>
+      <c r="F23">
+        <v>6.5699999999999995E-2</v>
+      </c>
+      <c r="G23">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>253</v>
+      </c>
+      <c r="B24">
+        <v>3.49E-2</v>
+      </c>
+      <c r="C24">
+        <v>3.3599999999999998E-2</v>
+      </c>
+      <c r="D24">
+        <v>3.5700000000000003E-2</v>
+      </c>
+      <c r="E24">
+        <v>-2.0999999999999999E-3</v>
+      </c>
+      <c r="F24">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="G24">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>254</v>
+      </c>
+      <c r="B25">
+        <v>5.3625999999999996</v>
+      </c>
+      <c r="C25">
+        <v>6.6986999999999997</v>
+      </c>
+      <c r="D25">
+        <v>4.8350999999999997</v>
+      </c>
+      <c r="E25">
+        <v>1.8635999999999999</v>
+      </c>
+      <c r="F25">
+        <v>3.4990000000000001</v>
+      </c>
+      <c r="G25">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>255</v>
+      </c>
+      <c r="B26">
+        <v>5.8900000000000001E-2</v>
+      </c>
+      <c r="C26">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="D26">
+        <v>5.6500000000000002E-2</v>
+      </c>
+      <c r="E26">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F26">
+        <v>5.4899999999999997E-2</v>
+      </c>
+      <c r="G26">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>239</v>
+      </c>
+      <c r="C27" t="s">
+        <v>240</v>
+      </c>
+      <c r="D27" t="s">
+        <v>241</v>
+      </c>
+      <c r="E27" t="s">
+        <v>242</v>
+      </c>
+      <c r="F27" t="s">
+        <v>243</v>
+      </c>
+      <c r="G27" t="s">
         <v>244</v>
       </c>
-      <c r="D62" t="s">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>245</v>
+      </c>
+      <c r="B28">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="C28">
+        <v>0.83440000000000003</v>
+      </c>
+      <c r="D28">
+        <v>0.82110000000000005</v>
+      </c>
+      <c r="E28">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="F28">
+        <v>0.81469999999999998</v>
+      </c>
+      <c r="G28">
+        <v>500</v>
+      </c>
+      <c r="H28">
+        <f>0.5*(F28+1)</f>
+        <v>0.90734999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>246</v>
+      </c>
+      <c r="B29">
+        <v>0.51529999999999998</v>
+      </c>
+      <c r="C29">
+        <v>0.52610000000000001</v>
+      </c>
+      <c r="D29">
+        <v>0.50419999999999998</v>
+      </c>
+      <c r="E29">
+        <v>2.18E-2</v>
+      </c>
+      <c r="F29">
+        <v>0.49349999999999999</v>
+      </c>
+      <c r="G29">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>247</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>-4.7E-2</v>
+      </c>
+      <c r="E30">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F30">
+        <v>-4.7E-2</v>
+      </c>
+      <c r="G30">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>248</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0.91</v>
+      </c>
+      <c r="E31">
+        <v>0.09</v>
+      </c>
+      <c r="F31">
+        <v>0.91</v>
+      </c>
+      <c r="G31">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>249</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>2.8899999999999999E-2</v>
+      </c>
+      <c r="E32">
+        <v>2.8899999999999999E-2</v>
+      </c>
+      <c r="F32">
+        <v>2.8899999999999999E-2</v>
+      </c>
+      <c r="G32">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>250</v>
+      </c>
+      <c r="B33">
+        <v>0.3518</v>
+      </c>
+      <c r="C33">
+        <v>0.3604</v>
+      </c>
+      <c r="D33">
+        <v>0.34279999999999999</v>
+      </c>
+      <c r="E33">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="F33">
+        <v>0.3342</v>
+      </c>
+      <c r="G33">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>251</v>
+      </c>
+      <c r="B34">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="C34">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="D34">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="E34">
+        <v>-2.5999999999999999E-3</v>
+      </c>
+      <c r="F34">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="G34">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>252</v>
       </c>
-      <c r="E62" t="s">
-        <v>36</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="B35">
+        <v>0.3533</v>
+      </c>
+      <c r="C35">
+        <v>0.3619</v>
+      </c>
+      <c r="D35">
+        <v>0.3417</v>
+      </c>
+      <c r="E35">
+        <v>2.0199999999999999E-2</v>
+      </c>
+      <c r="F35">
+        <v>0.33310000000000001</v>
+      </c>
+      <c r="G35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>253</v>
+      </c>
+      <c r="B36">
+        <v>8.3599999999999994E-2</v>
+      </c>
+      <c r="C36">
+        <v>8.1600000000000006E-2</v>
+      </c>
+      <c r="D36">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E36">
+        <v>-3.7000000000000002E-3</v>
+      </c>
+      <c r="F36">
+        <v>8.7300000000000003E-2</v>
+      </c>
+      <c r="G36">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>254</v>
+      </c>
+      <c r="B37">
+        <v>4.6203000000000003</v>
+      </c>
+      <c r="C37">
+        <v>4.8997999999999999</v>
+      </c>
+      <c r="D37">
+        <v>4.4211999999999998</v>
+      </c>
+      <c r="E37">
+        <v>0.47849999999999998</v>
+      </c>
+      <c r="F37">
+        <v>4.1417000000000002</v>
+      </c>
+      <c r="G37">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>255</v>
+      </c>
+      <c r="B38">
+        <v>0.21490000000000001</v>
+      </c>
+      <c r="C38">
+        <v>0.21609999999999999</v>
+      </c>
+      <c r="D38">
+        <v>0.21279999999999999</v>
+      </c>
+      <c r="E38">
+        <v>3.3E-3</v>
+      </c>
+      <c r="F38">
+        <v>0.21149999999999999</v>
+      </c>
+      <c r="G38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>239</v>
+      </c>
+      <c r="C39" t="s">
+        <v>240</v>
+      </c>
+      <c r="D39" t="s">
+        <v>241</v>
+      </c>
+      <c r="E39" t="s">
+        <v>242</v>
+      </c>
+      <c r="F39" t="s">
+        <v>243</v>
+      </c>
+      <c r="G39" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>245</v>
+      </c>
+      <c r="B40">
+        <v>0.71220000000000006</v>
+      </c>
+      <c r="C40">
+        <v>0.72950000000000004</v>
+      </c>
+      <c r="D40">
+        <v>0.69520000000000004</v>
+      </c>
+      <c r="E40">
+        <v>3.4299999999999997E-2</v>
+      </c>
+      <c r="F40">
+        <v>0.67779999999999996</v>
+      </c>
+      <c r="G40">
+        <v>500</v>
+      </c>
+      <c r="H40">
+        <f>0.5*(F40+1)</f>
+        <v>0.83889999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>246</v>
       </c>
-      <c r="G62" t="s">
+      <c r="B41">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="C41">
+        <v>0.28449999999999998</v>
+      </c>
+      <c r="D41">
+        <v>0.2402</v>
+      </c>
+      <c r="E41">
+        <v>4.4299999999999999E-2</v>
+      </c>
+      <c r="F41">
+        <v>0.2167</v>
+      </c>
+      <c r="G41">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>247</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>-0.29120000000000001</v>
+      </c>
+      <c r="E42">
+        <v>0.29120000000000001</v>
+      </c>
+      <c r="F42">
+        <v>-0.29120000000000001</v>
+      </c>
+      <c r="G42">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>248</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>0.85740000000000005</v>
+      </c>
+      <c r="E43">
+        <v>0.1426</v>
+      </c>
+      <c r="F43">
+        <v>0.85740000000000005</v>
+      </c>
+      <c r="G43">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>249</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>9.3200000000000005E-2</v>
+      </c>
+      <c r="E44">
+        <v>9.3200000000000005E-2</v>
+      </c>
+      <c r="F44">
+        <v>9.3200000000000005E-2</v>
+      </c>
+      <c r="G44">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>250</v>
+      </c>
+      <c r="B45">
+        <v>9.4600000000000004E-2</v>
+      </c>
+      <c r="C45">
+        <v>0.1037</v>
+      </c>
+      <c r="D45">
+        <v>8.6699999999999999E-2</v>
+      </c>
+      <c r="E45">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F45">
+        <v>7.7600000000000002E-2</v>
+      </c>
+      <c r="G45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>251</v>
+      </c>
+      <c r="B46">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="C46">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="D46">
+        <v>1.8E-3</v>
+      </c>
+      <c r="E46">
+        <v>-3.3E-3</v>
+      </c>
+      <c r="F46">
+        <v>1.8E-3</v>
+      </c>
+      <c r="G46">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>252</v>
+      </c>
+      <c r="B47">
+        <v>9.6100000000000005E-2</v>
+      </c>
+      <c r="C47">
+        <v>0.1052</v>
+      </c>
+      <c r="D47">
+        <v>8.4900000000000003E-2</v>
+      </c>
+      <c r="E47">
+        <v>2.0299999999999999E-2</v>
+      </c>
+      <c r="F47">
+        <v>7.5800000000000006E-2</v>
+      </c>
+      <c r="G47">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>0.9</v>
-      </c>
-      <c r="B63" t="s">
-        <v>248</v>
-      </c>
-      <c r="C63" t="s">
-        <v>249</v>
-      </c>
-      <c r="D63" t="s">
-        <v>244</v>
-      </c>
-      <c r="E63" t="s">
+      <c r="B48">
+        <v>4.6600000000000003E-2</v>
+      </c>
+      <c r="C48">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="D48">
+        <v>4.7399999999999998E-2</v>
+      </c>
+      <c r="E48">
+        <v>-2.3E-3</v>
+      </c>
+      <c r="F48">
+        <v>4.8899999999999999E-2</v>
+      </c>
+      <c r="G48">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="B49">
+        <v>2.2484000000000002</v>
+      </c>
+      <c r="C49">
+        <v>2.4174000000000002</v>
+      </c>
+      <c r="D49">
+        <v>2.0526</v>
+      </c>
+      <c r="E49">
+        <v>0.36480000000000001</v>
+      </c>
+      <c r="F49">
+        <v>1.8835999999999999</v>
+      </c>
+      <c r="G49">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>255</v>
       </c>
-      <c r="B66" t="s">
-        <v>36</v>
-      </c>
-      <c r="C66" t="s">
-        <v>244</v>
-      </c>
-      <c r="D66" t="s">
-        <v>256</v>
-      </c>
-      <c r="E66" t="s">
-        <v>36</v>
-      </c>
-      <c r="F66" t="s">
-        <v>246</v>
-      </c>
-      <c r="G66" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>0.9</v>
-      </c>
-      <c r="B67" t="s">
-        <v>248</v>
-      </c>
-      <c r="C67" t="s">
-        <v>249</v>
-      </c>
-      <c r="D67" t="s">
-        <v>244</v>
-      </c>
-      <c r="E67" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>259</v>
-      </c>
-      <c r="B70" t="s">
-        <v>36</v>
-      </c>
-      <c r="C70" t="s">
-        <v>244</v>
-      </c>
-      <c r="D70" t="s">
-        <v>260</v>
-      </c>
-      <c r="E70" t="s">
-        <v>36</v>
-      </c>
-      <c r="F70" t="s">
-        <v>246</v>
-      </c>
-      <c r="G70" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>0.9</v>
-      </c>
-      <c r="B71" t="s">
-        <v>248</v>
-      </c>
-      <c r="C71" t="s">
-        <v>249</v>
-      </c>
-      <c r="D71" t="s">
-        <v>244</v>
-      </c>
-      <c r="E71" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>243</v>
-      </c>
-      <c r="B74" t="s">
-        <v>36</v>
-      </c>
-      <c r="C74" t="s">
-        <v>244</v>
-      </c>
-      <c r="D74" t="s">
-        <v>263</v>
-      </c>
-      <c r="E74" t="s">
-        <v>36</v>
-      </c>
-      <c r="F74" t="s">
-        <v>246</v>
-      </c>
-      <c r="G74" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>0.9</v>
-      </c>
-      <c r="B75" t="s">
-        <v>248</v>
-      </c>
-      <c r="C75" t="s">
-        <v>249</v>
-      </c>
-      <c r="D75" t="s">
-        <v>244</v>
-      </c>
-      <c r="E75" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>251</v>
-      </c>
-      <c r="B78" t="s">
-        <v>36</v>
-      </c>
-      <c r="C78" t="s">
-        <v>244</v>
-      </c>
-      <c r="D78" t="s">
-        <v>266</v>
-      </c>
-      <c r="E78" t="s">
-        <v>36</v>
-      </c>
-      <c r="F78" t="s">
-        <v>246</v>
-      </c>
-      <c r="G78" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>0.9</v>
-      </c>
-      <c r="B79" t="s">
-        <v>248</v>
-      </c>
-      <c r="C79" t="s">
-        <v>249</v>
-      </c>
-      <c r="D79" t="s">
-        <v>244</v>
-      </c>
-      <c r="E79" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>255</v>
-      </c>
-      <c r="B82" t="s">
-        <v>36</v>
-      </c>
-      <c r="C82" t="s">
-        <v>244</v>
-      </c>
-      <c r="D82" t="s">
-        <v>269</v>
-      </c>
-      <c r="E82" t="s">
-        <v>36</v>
-      </c>
-      <c r="F82" t="s">
-        <v>246</v>
-      </c>
-      <c r="G82" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>0.9</v>
-      </c>
-      <c r="B83" t="s">
-        <v>248</v>
-      </c>
-      <c r="C83" t="s">
-        <v>249</v>
-      </c>
-      <c r="D83" t="s">
-        <v>244</v>
-      </c>
-      <c r="E83" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>259</v>
-      </c>
-      <c r="B86" t="s">
-        <v>36</v>
-      </c>
-      <c r="C86" t="s">
-        <v>244</v>
-      </c>
-      <c r="D86" t="s">
-        <v>272</v>
-      </c>
-      <c r="E86" t="s">
-        <v>36</v>
-      </c>
-      <c r="F86" t="s">
-        <v>246</v>
-      </c>
-      <c r="G86" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>0.9</v>
-      </c>
-      <c r="B87" t="s">
-        <v>248</v>
-      </c>
-      <c r="C87" t="s">
-        <v>249</v>
-      </c>
-      <c r="D87" t="s">
-        <v>244</v>
-      </c>
-      <c r="E87" t="s">
-        <v>266</v>
+      <c r="B50">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="C50">
+        <v>7.5300000000000006E-2</v>
+      </c>
+      <c r="D50">
+        <v>7.0300000000000001E-2</v>
+      </c>
+      <c r="E50">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F50">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="G50">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed T1D dur from DPN, AN, and DN models to improve model interpretability
</commit_message>
<xml_diff>
--- a/Diabetic_complications_tables.xlsx
+++ b/Diabetic_complications_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paultran/Box/Students/T1D_complications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F56D24-0AEC-804E-9822-79F326C19343}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02EF1CA-41F5-E240-808F-60172840FB01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17080" yWindow="1180" windowWidth="16520" windowHeight="16940" firstSheet="5" activeTab="7" xr2:uid="{D1842A1F-FBE3-7248-88B5-8CE7C8CE474E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="322">
   <si>
     <t>Peripheral_Neuropathy3</t>
   </si>
@@ -924,6 +924,81 @@
   </si>
   <si>
     <t xml:space="preserve">5.634497e+01 1.600000e+01 2.134086e-06 </t>
+  </si>
+  <si>
+    <t>n=1335   Mean absolute error=0.009   Mean squared error=0.00022</t>
+  </si>
+  <si>
+    <t>0.9 Quantile of absolute error=0.03</t>
+  </si>
+  <si>
+    <t>&gt; plot(rms::calibrate(bANselect, method="boot", B=500), las=1)</t>
+  </si>
+  <si>
+    <t>Divergence or singularity in 29 samples</t>
+  </si>
+  <si>
+    <t>n=1332   Mean absolute error=0.004   Mean squared error=6e-05</t>
+  </si>
+  <si>
+    <t>0.9 Quantile of absolute error=0.008</t>
+  </si>
+  <si>
+    <t>&gt; plot(rms::calibrate(bDNselect, method="boot", B=500), las=1)</t>
+  </si>
+  <si>
+    <t>n=1334   Mean absolute error=0.005   Mean squared error=0.00024</t>
+  </si>
+  <si>
+    <t>&gt; plot(rms::calibrate(bDPNselect, method="boot", B=500), las=1)</t>
+  </si>
+  <si>
+    <t>no dur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 1: Peripheral_Neuropathy3 ~ rcs(Dr_Age, 3) + Dur + avg.Systolic + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 2: Peripheral_Neuropathy3 ~ rcs(Dr_Age, 3) + avg.Systolic + rcs(Dx_Age, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    5) + rcs(AvgA1c, 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.1512043  1.0000000  0.2832972 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 1: Autonomic_Neuropathy3 ~ rcs(Dr_Age, 3) + Dur + rcs(Dx_Age, 5) + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 2: Autonomic_Neuropathy3 ~ rcs(Dr_Age, 3) + rcs(Dx_Age, 5) + avg.Systolic + </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.1559297  1.0000000  0.2823113 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 1: DM_Retinopathy3 ~ rcs(Dr_Age, 3) + rcs(Dur, 3) + rcs(Dx_Age, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 2: DM_Retinopathy3 ~ rcs(Dr_Age, 3) + rcs(Dx_Age, 5) + avg.Systolic + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.599532e+01 2.000000e+00 3.362483e-04 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 1: DM_Nephropathy3 ~ rcs(Dr_Age, 3) + Dur + rcs(Dx_Age, 5) + avg.Systolic + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 2: DM_Nephropathy3 ~ rcs(Dr_Age, 3) + rcs(Dx_Age, 5) + avg.Systolic + </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.2471913  1.0000000  0.0393153 </t>
+  </si>
+  <si>
+    <t>full vs preselected</t>
+  </si>
+  <si>
+    <t>preselected vs rm dur</t>
   </si>
 </sst>
 </file>
@@ -1149,6 +1224,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1167,7 +1243,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6078,26 +6153,26 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="23"/>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41" t="s">
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41" t="s">
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
     </row>
     <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="23" t="s">
@@ -9108,26 +9183,26 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="45" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="46"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45" t="s">
+      <c r="F2" s="47"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="46"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="45" t="s">
+      <c r="I2" s="47"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="46"/>
-      <c r="M2" s="44"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="45"/>
       <c r="N2" s="12"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -10414,10 +10489,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1880468A-055E-BA41-A377-B9D926328429}">
-  <dimension ref="A1:K109"/>
+  <dimension ref="A1:P109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" topLeftCell="F41" workbookViewId="0">
+      <selection activeCell="P63" sqref="P63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11512,7 +11587,7 @@
         <v>0.80035000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>236</v>
       </c>
@@ -11541,7 +11616,7 @@
         <v>2.2263000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>41</v>
       </c>
@@ -11567,7 +11642,7 @@
         <v>7.6572999999999997E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>236</v>
       </c>
@@ -11596,7 +11671,7 @@
         <v>1.0077</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>51</v>
       </c>
@@ -11622,7 +11697,7 @@
         <v>0.94340000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>236</v>
       </c>
@@ -11651,7 +11726,7 @@
         <v>2.5687000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>54</v>
       </c>
@@ -11677,7 +11752,7 @@
         <v>1.0064</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>236</v>
       </c>
@@ -11706,33 +11781,53 @@
         <v>2.7357999999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H58" t="s">
+        <v>320</v>
+      </c>
+      <c r="P58" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>263</v>
       </c>
       <c r="H60" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P60" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>264</v>
       </c>
       <c r="H61" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P61" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H62" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P62" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H63" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P63" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>265</v>
       </c>
@@ -11740,20 +11835,26 @@
         <v>276</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H65" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="P65" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>266</v>
       </c>
       <c r="H66" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="P66" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>267</v>
       </c>
@@ -11761,126 +11862,218 @@
         <v>279</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H69" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="P69" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>268</v>
       </c>
       <c r="H70" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="P70" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="P71" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P72" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H73" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>270</v>
       </c>
       <c r="H74" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="P74" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>271</v>
       </c>
       <c r="H75" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="P75" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H76" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H77" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H78" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="P78" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>305</v>
+      </c>
       <c r="H79" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="P79" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H80" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="82" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="P80" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>297</v>
+      </c>
+      <c r="P81" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>298</v>
+      </c>
       <c r="H82" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="83" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H83" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="86" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="P83" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>299</v>
+      </c>
+      <c r="P84" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>300</v>
+      </c>
       <c r="H86" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="87" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H87" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="88" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="P87" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>301</v>
+      </c>
       <c r="H88" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="89" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="P88" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>302</v>
+      </c>
       <c r="H89" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="90" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="P89" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H90" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="91" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="P90" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>303</v>
+      </c>
       <c r="H91" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="92" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H92" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="93" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="P92" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>304</v>
+      </c>
       <c r="H93" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="95" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="P93" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H95" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="96" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H96" t="s">
         <v>290</v>
       </c>
@@ -11942,10 +12135,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2987885-C709-614F-8DFD-D0F729A65828}">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11999,7 +12192,7 @@
         <f>0.5*(F2+1)</f>
         <v>0.87345000000000006</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="41" t="s">
         <v>261</v>
       </c>
     </row>
@@ -13038,7 +13231,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>254</v>
       </c>
@@ -13061,7 +13254,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>255</v>
       </c>
@@ -13081,6 +13274,1157 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="G50">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>239</v>
+      </c>
+      <c r="C55" t="s">
+        <v>240</v>
+      </c>
+      <c r="D55" t="s">
+        <v>241</v>
+      </c>
+      <c r="E55" t="s">
+        <v>242</v>
+      </c>
+      <c r="F55" t="s">
+        <v>243</v>
+      </c>
+      <c r="G55" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>245</v>
+      </c>
+      <c r="B56">
+        <v>0.76180000000000003</v>
+      </c>
+      <c r="C56">
+        <v>0.77159999999999995</v>
+      </c>
+      <c r="D56">
+        <v>0.75570000000000004</v>
+      </c>
+      <c r="E56">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="F56">
+        <v>0.74590000000000001</v>
+      </c>
+      <c r="G56">
+        <v>500</v>
+      </c>
+      <c r="H56">
+        <f>0.5*(F56+1)</f>
+        <v>0.87295</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>246</v>
+      </c>
+      <c r="B57">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="C57">
+        <v>0.42</v>
+      </c>
+      <c r="D57">
+        <v>0.39850000000000002</v>
+      </c>
+      <c r="E57">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="F57">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="G57">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>247</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>-7.1499999999999994E-2</v>
+      </c>
+      <c r="E58">
+        <v>7.1499999999999994E-2</v>
+      </c>
+      <c r="F58">
+        <v>-7.1499999999999994E-2</v>
+      </c>
+      <c r="G58">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>248</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>0.92720000000000002</v>
+      </c>
+      <c r="E59">
+        <v>7.2800000000000004E-2</v>
+      </c>
+      <c r="F59">
+        <v>0.92720000000000002</v>
+      </c>
+      <c r="G59">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>249</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>2.9499999999999998E-2</v>
+      </c>
+      <c r="E60">
+        <v>2.9499999999999998E-2</v>
+      </c>
+      <c r="F60">
+        <v>2.9499999999999998E-2</v>
+      </c>
+      <c r="G60">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>250</v>
+      </c>
+      <c r="B61">
+        <v>0.2462</v>
+      </c>
+      <c r="C61">
+        <v>0.25340000000000001</v>
+      </c>
+      <c r="D61">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="E61">
+        <v>1.44E-2</v>
+      </c>
+      <c r="F61">
+        <v>0.23169999999999999</v>
+      </c>
+      <c r="G61">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>251</v>
+      </c>
+      <c r="B62">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="C62">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="D62">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="E62">
+        <v>-2.3E-3</v>
+      </c>
+      <c r="F62">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="G62">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>252</v>
+      </c>
+      <c r="B63">
+        <v>0.2477</v>
+      </c>
+      <c r="C63">
+        <v>0.25490000000000002</v>
+      </c>
+      <c r="D63">
+        <v>0.2382</v>
+      </c>
+      <c r="E63">
+        <v>1.67E-2</v>
+      </c>
+      <c r="F63">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="G63">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>253</v>
+      </c>
+      <c r="B64">
+        <v>8.3400000000000002E-2</v>
+      </c>
+      <c r="C64">
+        <v>8.1600000000000006E-2</v>
+      </c>
+      <c r="D64">
+        <v>8.48E-2</v>
+      </c>
+      <c r="E64">
+        <v>-3.2000000000000002E-3</v>
+      </c>
+      <c r="F64">
+        <v>8.6599999999999996E-2</v>
+      </c>
+      <c r="G64">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>254</v>
+      </c>
+      <c r="B65">
+        <v>2.9952000000000001</v>
+      </c>
+      <c r="C65">
+        <v>3.1564000000000001</v>
+      </c>
+      <c r="D65">
+        <v>2.9020000000000001</v>
+      </c>
+      <c r="E65">
+        <v>0.25440000000000002</v>
+      </c>
+      <c r="F65">
+        <v>2.7408000000000001</v>
+      </c>
+      <c r="G65">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>255</v>
+      </c>
+      <c r="B66">
+        <v>0.1709</v>
+      </c>
+      <c r="C66">
+        <v>0.1721</v>
+      </c>
+      <c r="D66">
+        <v>0.16880000000000001</v>
+      </c>
+      <c r="E66">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="F66">
+        <v>0.16769999999999999</v>
+      </c>
+      <c r="G66">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>256</v>
+      </c>
+      <c r="B68" t="s">
+        <v>257</v>
+      </c>
+      <c r="C68" t="s">
+        <v>258</v>
+      </c>
+      <c r="D68" t="s">
+        <v>259</v>
+      </c>
+      <c r="E68">
+        <v>22</v>
+      </c>
+      <c r="F68" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>239</v>
+      </c>
+      <c r="C69" t="s">
+        <v>240</v>
+      </c>
+      <c r="D69" t="s">
+        <v>241</v>
+      </c>
+      <c r="E69" t="s">
+        <v>242</v>
+      </c>
+      <c r="F69" t="s">
+        <v>243</v>
+      </c>
+      <c r="G69" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>245</v>
+      </c>
+      <c r="B70">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="C70">
+        <v>0.77659999999999996</v>
+      </c>
+      <c r="D70">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="E70">
+        <v>3.8600000000000002E-2</v>
+      </c>
+      <c r="F70">
+        <v>0.72240000000000004</v>
+      </c>
+      <c r="G70">
+        <v>478</v>
+      </c>
+      <c r="H70">
+        <f>0.5*(F70+1)</f>
+        <v>0.86119999999999997</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>246</v>
+      </c>
+      <c r="B71">
+        <v>0.28510000000000002</v>
+      </c>
+      <c r="C71">
+        <v>0.3085</v>
+      </c>
+      <c r="D71">
+        <v>0.26450000000000001</v>
+      </c>
+      <c r="E71">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F71">
+        <v>0.24110000000000001</v>
+      </c>
+      <c r="G71">
+        <v>478</v>
+      </c>
+      <c r="I71" s="40"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>247</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>-0.44409999999999999</v>
+      </c>
+      <c r="E72">
+        <v>0.44409999999999999</v>
+      </c>
+      <c r="F72">
+        <v>-0.44409999999999999</v>
+      </c>
+      <c r="G72">
+        <v>478</v>
+      </c>
+      <c r="J72" s="40"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>248</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>0.79039999999999999</v>
+      </c>
+      <c r="E73">
+        <v>0.20960000000000001</v>
+      </c>
+      <c r="F73">
+        <v>0.79039999999999999</v>
+      </c>
+      <c r="G73">
+        <v>478</v>
+      </c>
+      <c r="I73" s="40"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>249</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0.14549999999999999</v>
+      </c>
+      <c r="E74">
+        <v>0.14549999999999999</v>
+      </c>
+      <c r="F74">
+        <v>0.14549999999999999</v>
+      </c>
+      <c r="G74">
+        <v>478</v>
+      </c>
+      <c r="J74" s="40"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>250</v>
+      </c>
+      <c r="B75">
+        <v>8.48E-2</v>
+      </c>
+      <c r="C75">
+        <v>9.2799999999999994E-2</v>
+      </c>
+      <c r="D75">
+        <v>7.8399999999999997E-2</v>
+      </c>
+      <c r="E75">
+        <v>1.44E-2</v>
+      </c>
+      <c r="F75">
+        <v>7.0499999999999993E-2</v>
+      </c>
+      <c r="G75">
+        <v>478</v>
+      </c>
+      <c r="I75" s="40"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>251</v>
+      </c>
+      <c r="B76">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="C76">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="D76">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="E76">
+        <v>-3.8999999999999998E-3</v>
+      </c>
+      <c r="F76">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="G76">
+        <v>478</v>
+      </c>
+      <c r="J76" s="40"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>252</v>
+      </c>
+      <c r="B77">
+        <v>8.6300000000000002E-2</v>
+      </c>
+      <c r="C77">
+        <v>9.4299999999999995E-2</v>
+      </c>
+      <c r="D77">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="E77">
+        <v>1.83E-2</v>
+      </c>
+      <c r="F77">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="G77">
+        <v>478</v>
+      </c>
+      <c r="I77" s="40"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>253</v>
+      </c>
+      <c r="B78">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C78">
+        <v>3.44E-2</v>
+      </c>
+      <c r="D78">
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="E78">
+        <v>-1.4E-3</v>
+      </c>
+      <c r="F78">
+        <v>3.6400000000000002E-2</v>
+      </c>
+      <c r="G78">
+        <v>478</v>
+      </c>
+      <c r="J78" s="40"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>254</v>
+      </c>
+      <c r="B79">
+        <v>5.3853</v>
+      </c>
+      <c r="C79">
+        <v>6.8411</v>
+      </c>
+      <c r="D79">
+        <v>5.1566999999999998</v>
+      </c>
+      <c r="E79">
+        <v>1.6842999999999999</v>
+      </c>
+      <c r="F79">
+        <v>3.7010000000000001</v>
+      </c>
+      <c r="G79">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>255</v>
+      </c>
+      <c r="B80">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="C80">
+        <v>6.0600000000000001E-2</v>
+      </c>
+      <c r="D80">
+        <v>5.67E-2</v>
+      </c>
+      <c r="E80">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="F80">
+        <v>5.4800000000000001E-2</v>
+      </c>
+      <c r="G80">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>239</v>
+      </c>
+      <c r="C81" t="s">
+        <v>240</v>
+      </c>
+      <c r="D81" t="s">
+        <v>241</v>
+      </c>
+      <c r="E81" t="s">
+        <v>242</v>
+      </c>
+      <c r="F81" t="s">
+        <v>243</v>
+      </c>
+      <c r="G81" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>245</v>
+      </c>
+      <c r="B82">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="C82">
+        <v>0.83420000000000005</v>
+      </c>
+      <c r="D82">
+        <v>0.82120000000000004</v>
+      </c>
+      <c r="E82">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F82">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="G82">
+        <v>500</v>
+      </c>
+      <c r="H82">
+        <f>0.5*(F82+1)</f>
+        <v>0.90749999999999997</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>246</v>
+      </c>
+      <c r="B83">
+        <v>0.51529999999999998</v>
+      </c>
+      <c r="C83">
+        <v>0.52639999999999998</v>
+      </c>
+      <c r="D83">
+        <v>0.50439999999999996</v>
+      </c>
+      <c r="E83">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F83">
+        <v>0.49320000000000003</v>
+      </c>
+      <c r="G83">
+        <v>500</v>
+      </c>
+      <c r="I83" s="40"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>247</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>-5.5100000000000003E-2</v>
+      </c>
+      <c r="E84">
+        <v>5.5100000000000003E-2</v>
+      </c>
+      <c r="F84">
+        <v>-5.5100000000000003E-2</v>
+      </c>
+      <c r="G84">
+        <v>500</v>
+      </c>
+      <c r="J84" s="40"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>248</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>0.91449999999999998</v>
+      </c>
+      <c r="E85">
+        <v>8.5500000000000007E-2</v>
+      </c>
+      <c r="F85">
+        <v>0.91449999999999998</v>
+      </c>
+      <c r="G85">
+        <v>500</v>
+      </c>
+      <c r="I85" s="40"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>249</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>2.93E-2</v>
+      </c>
+      <c r="E86">
+        <v>2.93E-2</v>
+      </c>
+      <c r="F86">
+        <v>2.93E-2</v>
+      </c>
+      <c r="G86">
+        <v>500</v>
+      </c>
+      <c r="J86" s="40"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>250</v>
+      </c>
+      <c r="B87">
+        <v>0.3518</v>
+      </c>
+      <c r="C87">
+        <v>0.3614</v>
+      </c>
+      <c r="D87">
+        <v>0.34289999999999998</v>
+      </c>
+      <c r="E87">
+        <v>1.8599999999999998E-2</v>
+      </c>
+      <c r="F87">
+        <v>0.3332</v>
+      </c>
+      <c r="G87">
+        <v>500</v>
+      </c>
+      <c r="I87" s="40"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>251</v>
+      </c>
+      <c r="B88">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="C88">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="D88">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="E88">
+        <v>-2.8E-3</v>
+      </c>
+      <c r="F88">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="G88">
+        <v>500</v>
+      </c>
+      <c r="J88" s="40"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>252</v>
+      </c>
+      <c r="B89">
+        <v>0.3533</v>
+      </c>
+      <c r="C89">
+        <v>0.3629</v>
+      </c>
+      <c r="D89">
+        <v>0.34160000000000001</v>
+      </c>
+      <c r="E89">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="F89">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="G89">
+        <v>500</v>
+      </c>
+      <c r="I89" s="40"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>253</v>
+      </c>
+      <c r="B90">
+        <v>8.3599999999999994E-2</v>
+      </c>
+      <c r="C90">
+        <v>8.1799999999999998E-2</v>
+      </c>
+      <c r="D90">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E90">
+        <v>-3.5000000000000001E-3</v>
+      </c>
+      <c r="F90">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="G90">
+        <v>500</v>
+      </c>
+      <c r="J90" s="40"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>254</v>
+      </c>
+      <c r="B91">
+        <v>4.6203000000000003</v>
+      </c>
+      <c r="C91">
+        <v>4.9176000000000002</v>
+      </c>
+      <c r="D91">
+        <v>4.4581999999999997</v>
+      </c>
+      <c r="E91">
+        <v>0.45929999999999999</v>
+      </c>
+      <c r="F91">
+        <v>4.1608999999999998</v>
+      </c>
+      <c r="G91">
+        <v>500</v>
+      </c>
+      <c r="I91" s="40"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>255</v>
+      </c>
+      <c r="B92">
+        <v>0.21490000000000001</v>
+      </c>
+      <c r="C92">
+        <v>0.21679999999999999</v>
+      </c>
+      <c r="D92">
+        <v>0.21279999999999999</v>
+      </c>
+      <c r="E92">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F92">
+        <v>0.21079999999999999</v>
+      </c>
+      <c r="G92">
+        <v>500</v>
+      </c>
+      <c r="J92" s="40"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>239</v>
+      </c>
+      <c r="C93" t="s">
+        <v>240</v>
+      </c>
+      <c r="D93" t="s">
+        <v>241</v>
+      </c>
+      <c r="E93" t="s">
+        <v>242</v>
+      </c>
+      <c r="F93" t="s">
+        <v>243</v>
+      </c>
+      <c r="G93" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>245</v>
+      </c>
+      <c r="B94">
+        <v>0.7006</v>
+      </c>
+      <c r="C94">
+        <v>0.71460000000000001</v>
+      </c>
+      <c r="D94">
+        <v>0.6794</v>
+      </c>
+      <c r="E94">
+        <v>3.5200000000000002E-2</v>
+      </c>
+      <c r="F94">
+        <v>0.66549999999999998</v>
+      </c>
+      <c r="G94">
+        <v>500</v>
+      </c>
+      <c r="H94">
+        <f>0.5*(F94+1)</f>
+        <v>0.83274999999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>246</v>
+      </c>
+      <c r="B95">
+        <v>0.25269999999999998</v>
+      </c>
+      <c r="C95">
+        <v>0.27210000000000001</v>
+      </c>
+      <c r="D95">
+        <v>0.23530000000000001</v>
+      </c>
+      <c r="E95">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="F95">
+        <v>0.21590000000000001</v>
+      </c>
+      <c r="G95">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>247</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>-0.24129999999999999</v>
+      </c>
+      <c r="E96">
+        <v>0.24129999999999999</v>
+      </c>
+      <c r="F96">
+        <v>-0.24129999999999999</v>
+      </c>
+      <c r="G96">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>248</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>0.88390000000000002</v>
+      </c>
+      <c r="E97">
+        <v>0.11609999999999999</v>
+      </c>
+      <c r="F97">
+        <v>0.88390000000000002</v>
+      </c>
+      <c r="G97">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>249</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>7.5800000000000006E-2</v>
+      </c>
+      <c r="E98">
+        <v>7.5800000000000006E-2</v>
+      </c>
+      <c r="F98">
+        <v>7.5800000000000006E-2</v>
+      </c>
+      <c r="G98">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>250</v>
+      </c>
+      <c r="B99">
+        <v>9.1499999999999998E-2</v>
+      </c>
+      <c r="C99">
+        <v>9.9299999999999999E-2</v>
+      </c>
+      <c r="D99">
+        <v>8.48E-2</v>
+      </c>
+      <c r="E99">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="F99">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="G99">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>251</v>
+      </c>
+      <c r="B100">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="C100">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="D100">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="E100">
+        <v>-2.7000000000000001E-3</v>
+      </c>
+      <c r="F100">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="G100">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>252</v>
+      </c>
+      <c r="B101">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="C101">
+        <v>0.1008</v>
+      </c>
+      <c r="D101">
+        <v>8.3599999999999994E-2</v>
+      </c>
+      <c r="E101">
+        <v>1.72E-2</v>
+      </c>
+      <c r="F101">
+        <v>7.5700000000000003E-2</v>
+      </c>
+      <c r="G101">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>253</v>
+      </c>
+      <c r="B102">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="C102">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D102">
+        <v>4.7800000000000002E-2</v>
+      </c>
+      <c r="E102">
+        <v>-1.8E-3</v>
+      </c>
+      <c r="F102">
+        <v>4.8599999999999997E-2</v>
+      </c>
+      <c r="G102">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>254</v>
+      </c>
+      <c r="B103">
+        <v>2.2427999999999999</v>
+      </c>
+      <c r="C103">
+        <v>2.4117999999999999</v>
+      </c>
+      <c r="D103">
+        <v>2.1006999999999998</v>
+      </c>
+      <c r="E103">
+        <v>0.31109999999999999</v>
+      </c>
+      <c r="F103">
+        <v>1.9317</v>
+      </c>
+      <c r="G103">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>255</v>
+      </c>
+      <c r="B104">
+        <v>7.2300000000000003E-2</v>
+      </c>
+      <c r="C104">
+        <v>7.46E-2</v>
+      </c>
+      <c r="D104">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E104">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="F104">
+        <v>6.7799999999999999E-2</v>
+      </c>
+      <c r="G104">
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change website name, modify methods, modify data tables, change CAD and PeriNeuro
</commit_message>
<xml_diff>
--- a/Diabetic_complications_tables.xlsx
+++ b/Diabetic_complications_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paultran/Box/Students/T1D_complications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02EF1CA-41F5-E240-808F-60172840FB01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1343FFF-E754-C04B-8933-81528B39CBC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17080" yWindow="1180" windowWidth="16520" windowHeight="16940" firstSheet="5" activeTab="7" xr2:uid="{D1842A1F-FBE3-7248-88B5-8CE7C8CE474E}"/>
+    <workbookView xWindow="9220" yWindow="1180" windowWidth="24380" windowHeight="16940" activeTab="3" xr2:uid="{D1842A1F-FBE3-7248-88B5-8CE7C8CE474E}"/>
   </bookViews>
   <sheets>
     <sheet name="table 1 raw" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="323">
   <si>
     <t>Peripheral_Neuropathy3</t>
   </si>
@@ -999,15 +999,19 @@
   </si>
   <si>
     <t>preselected vs rm dur</t>
+  </si>
+  <si>
+    <t>&lt;0.0001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1136,7 +1140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1241,6 +1245,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6112,24 +6125,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C558282E-B181-8C44-A5E0-7CFC83E81BA0}">
-  <dimension ref="A1:M68"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.5" style="30" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="50" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.1640625" style="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="50" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.1640625" style="32" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5" style="31" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="50" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.1640625" style="32" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.1640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" style="50" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="2.1640625" style="32" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="10.83203125" style="24"/>
   </cols>
@@ -6139,16 +6154,16 @@
         <v>104</v>
       </c>
       <c r="B1" s="18"/>
-      <c r="C1" s="19"/>
+      <c r="C1" s="48"/>
       <c r="D1" s="19"/>
       <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
+      <c r="F1" s="48"/>
       <c r="G1" s="19"/>
       <c r="H1" s="18"/>
-      <c r="I1" s="20"/>
+      <c r="I1" s="49"/>
       <c r="J1" s="20"/>
       <c r="K1" s="21"/>
-      <c r="L1" s="20"/>
+      <c r="L1" s="49"/>
       <c r="M1" s="20"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
@@ -6181,28 +6196,28 @@
       <c r="B3" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="48" t="s">
         <v>204</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="48" t="s">
         <v>204</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="48" t="s">
         <v>204</v>
       </c>
       <c r="J3" s="19"/>
       <c r="K3" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="48" t="s">
         <v>204</v>
       </c>
       <c r="M3" s="20"/>
@@ -6214,8 +6229,8 @@
       <c r="B4" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C4" s="27">
-        <v>2.4999999999999999E-49</v>
+      <c r="C4" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D4" s="27" t="s">
         <v>180</v>
@@ -6223,8 +6238,8 @@
       <c r="E4" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F4" s="27">
-        <v>6.7E-15</v>
+      <c r="F4" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="G4" s="27" t="s">
         <v>180</v>
@@ -6232,8 +6247,8 @@
       <c r="H4" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I4" s="27">
-        <v>4.9999999999999997E-50</v>
+      <c r="I4" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J4" s="27" t="s">
         <v>180</v>
@@ -6241,8 +6256,8 @@
       <c r="K4" s="26">
         <v>1</v>
       </c>
-      <c r="L4" s="27">
-        <v>2.8000000000000001E-16</v>
+      <c r="L4" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M4" s="27" t="s">
         <v>180</v>
@@ -6255,8 +6270,8 @@
       <c r="B5" s="26">
         <v>1</v>
       </c>
-      <c r="C5" s="27">
-        <v>9.7999999999999996E-22</v>
+      <c r="C5" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D5" s="27" t="s">
         <v>180</v>
@@ -6264,7 +6279,7 @@
       <c r="E5" s="26">
         <v>1</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="49">
         <v>1.5E-3</v>
       </c>
       <c r="G5" s="27" t="s">
@@ -6273,7 +6288,7 @@
       <c r="H5" s="26">
         <v>1</v>
       </c>
-      <c r="I5" s="27">
+      <c r="I5" s="49">
         <v>3.8999999999999998E-3</v>
       </c>
       <c r="J5" s="27" t="s">
@@ -6282,7 +6297,7 @@
       <c r="K5" s="26">
         <v>1</v>
       </c>
-      <c r="L5" s="27">
+      <c r="L5" s="49">
         <v>3.1E-2</v>
       </c>
       <c r="M5" s="27" t="s">
@@ -6296,8 +6311,8 @@
       <c r="B6" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C6" s="27">
-        <v>1.2999999999999999E-45</v>
+      <c r="C6" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D6" s="27" t="s">
         <v>180</v>
@@ -6305,8 +6320,8 @@
       <c r="E6" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F6" s="27">
-        <v>2.2E-16</v>
+      <c r="F6" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="G6" s="27" t="s">
         <v>180</v>
@@ -6314,8 +6329,8 @@
       <c r="H6" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I6" s="27">
-        <v>2.3E-65</v>
+      <c r="I6" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J6" s="27" t="s">
         <v>180</v>
@@ -6323,8 +6338,8 @@
       <c r="K6" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L6" s="27">
-        <v>7.8000000000000001E-21</v>
+      <c r="L6" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M6" s="27" t="s">
         <v>180</v>
@@ -6337,7 +6352,7 @@
       <c r="B7" s="26">
         <v>0.7</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="49">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D7" s="27" t="s">
@@ -6346,14 +6361,14 @@
       <c r="E7" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="49">
         <v>0.65</v>
       </c>
       <c r="G7" s="27"/>
       <c r="H7" s="26">
         <v>0.7</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7" s="49">
         <v>3.8E-3</v>
       </c>
       <c r="J7" s="27" t="s">
@@ -6362,7 +6377,7 @@
       <c r="K7" s="26">
         <v>0.9</v>
       </c>
-      <c r="L7" s="27">
+      <c r="L7" s="49">
         <v>0.48</v>
       </c>
       <c r="M7" s="27"/>
@@ -6370,16 +6385,16 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="23"/>
       <c r="B8" s="26"/>
-      <c r="C8" s="27"/>
+      <c r="C8" s="49"/>
       <c r="D8" s="27"/>
       <c r="E8" s="26"/>
-      <c r="F8" s="27"/>
+      <c r="F8" s="49"/>
       <c r="G8" s="27"/>
       <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
+      <c r="I8" s="49"/>
       <c r="J8" s="27"/>
       <c r="K8" s="26"/>
-      <c r="L8" s="27"/>
+      <c r="L8" s="49"/>
       <c r="M8" s="27"/>
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.15">
@@ -6387,16 +6402,16 @@
         <v>115</v>
       </c>
       <c r="B9" s="21"/>
-      <c r="C9" s="20"/>
+      <c r="C9" s="49"/>
       <c r="D9" s="27"/>
       <c r="E9" s="21"/>
-      <c r="F9" s="20"/>
+      <c r="F9" s="49"/>
       <c r="G9" s="27"/>
       <c r="H9" s="21"/>
-      <c r="I9" s="20"/>
+      <c r="I9" s="49"/>
       <c r="J9" s="27"/>
       <c r="K9" s="21"/>
-      <c r="L9" s="20"/>
+      <c r="L9" s="49"/>
       <c r="M9" s="27"/>
     </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.15">
@@ -6404,27 +6419,27 @@
         <v>117</v>
       </c>
       <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="27"/>
       <c r="E10" s="26">
         <v>25.4</v>
       </c>
-      <c r="F10" s="27">
-        <v>1.6E-27</v>
+      <c r="F10" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="G10" s="27"/>
       <c r="H10" s="26">
         <v>12.2</v>
       </c>
-      <c r="I10" s="27">
-        <v>4.7999999999999998E-49</v>
+      <c r="I10" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J10" s="27"/>
       <c r="K10" s="26">
         <v>7.9</v>
       </c>
-      <c r="L10" s="27">
-        <v>2.8E-19</v>
+      <c r="L10" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M10" s="27"/>
     </row>
@@ -6435,22 +6450,22 @@
       <c r="B11" s="26">
         <v>25.4</v>
       </c>
-      <c r="C11" s="27">
-        <v>1.6E-27</v>
+      <c r="C11" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D11" s="27" t="s">
         <v>180</v>
       </c>
       <c r="E11" s="26"/>
-      <c r="F11" s="27"/>
+      <c r="F11" s="49"/>
       <c r="G11" s="27" t="s">
         <v>180</v>
       </c>
       <c r="H11" s="26">
         <v>9.3000000000000007</v>
       </c>
-      <c r="I11" s="27">
-        <v>8.9999999999999996E-17</v>
+      <c r="I11" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J11" s="27" t="s">
         <v>180</v>
@@ -6458,8 +6473,8 @@
       <c r="K11" s="26">
         <v>6</v>
       </c>
-      <c r="L11" s="27">
-        <v>4.3000000000000001E-8</v>
+      <c r="L11" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M11" s="27" t="s">
         <v>180</v>
@@ -6472,8 +6487,8 @@
       <c r="B12" s="26">
         <v>12.2</v>
       </c>
-      <c r="C12" s="27">
-        <v>4.7999999999999998E-49</v>
+      <c r="C12" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>180</v>
@@ -6481,22 +6496,22 @@
       <c r="E12" s="26">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F12" s="27">
-        <v>8.9000000000000004E-17</v>
+      <c r="F12" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="G12" s="27" t="s">
         <v>180</v>
       </c>
       <c r="H12" s="26"/>
-      <c r="I12" s="27"/>
+      <c r="I12" s="49"/>
       <c r="J12" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K12" s="26">
         <v>13.7</v>
       </c>
-      <c r="L12" s="27">
-        <v>2.2E-28</v>
+      <c r="L12" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M12" s="27" t="s">
         <v>180</v>
@@ -6509,8 +6524,8 @@
       <c r="B13" s="26">
         <v>7.9</v>
       </c>
-      <c r="C13" s="27">
-        <v>2.8E-19</v>
+      <c r="C13" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D13" s="27" t="s">
         <v>180</v>
@@ -6518,8 +6533,8 @@
       <c r="E13" s="26">
         <v>6</v>
       </c>
-      <c r="F13" s="27">
-        <v>4.3000000000000001E-8</v>
+      <c r="F13" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="G13" s="27" t="s">
         <v>180</v>
@@ -6527,14 +6542,14 @@
       <c r="H13" s="26">
         <v>13.7</v>
       </c>
-      <c r="I13" s="27">
-        <v>2.2E-28</v>
+      <c r="I13" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J13" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K13" s="26"/>
-      <c r="L13" s="27"/>
+      <c r="L13" s="49"/>
       <c r="M13" s="27" t="s">
         <v>180</v>
       </c>
@@ -6546,8 +6561,8 @@
       <c r="B14" s="26">
         <v>6.6</v>
       </c>
-      <c r="C14" s="27">
-        <v>3.3999999999999998E-9</v>
+      <c r="C14" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D14" s="27" t="s">
         <v>180</v>
@@ -6555,8 +6570,8 @@
       <c r="E14" s="26">
         <v>5.6</v>
       </c>
-      <c r="F14" s="27">
-        <v>8.1000000000000004E-5</v>
+      <c r="F14" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="G14" s="27" t="s">
         <v>180</v>
@@ -6564,8 +6579,8 @@
       <c r="H14" s="26">
         <v>286</v>
       </c>
-      <c r="I14" s="27">
-        <v>2.4999999999999999E-8</v>
+      <c r="I14" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J14" s="27" t="s">
         <v>180</v>
@@ -6573,8 +6588,8 @@
       <c r="K14" s="26">
         <v>19.100000000000001</v>
       </c>
-      <c r="L14" s="27">
-        <v>1.8999999999999999E-18</v>
+      <c r="L14" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M14" s="27" t="s">
         <v>180</v>
@@ -6587,8 +6602,8 @@
       <c r="B15" s="26">
         <v>10.5</v>
       </c>
-      <c r="C15" s="27">
-        <v>6.6000000000000005E-38</v>
+      <c r="C15" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D15" s="27" t="s">
         <v>180</v>
@@ -6596,8 +6611,8 @@
       <c r="E15" s="26">
         <v>8.1</v>
       </c>
-      <c r="F15" s="27">
-        <v>1.4E-14</v>
+      <c r="F15" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="G15" s="27" t="s">
         <v>180</v>
@@ -6605,8 +6620,8 @@
       <c r="H15" s="26">
         <v>1492.5</v>
       </c>
-      <c r="I15" s="27">
-        <v>3.8000000000000003E-24</v>
+      <c r="I15" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J15" s="27" t="s">
         <v>180</v>
@@ -6614,8 +6629,8 @@
       <c r="K15" s="26">
         <v>14.5</v>
       </c>
-      <c r="L15" s="27">
-        <v>3.8000000000000003E-30</v>
+      <c r="L15" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M15" s="27" t="s">
         <v>180</v>
@@ -6628,8 +6643,8 @@
       <c r="B16" s="26">
         <v>36.200000000000003</v>
       </c>
-      <c r="C16" s="27">
-        <v>2.0999999999999999E-8</v>
+      <c r="C16" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D16" s="27" t="s">
         <v>180</v>
@@ -6637,8 +6652,8 @@
       <c r="E16" s="26">
         <v>11.4</v>
       </c>
-      <c r="F16" s="27">
-        <v>9.3000000000000007E-6</v>
+      <c r="F16" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="G16" s="27" t="s">
         <v>180</v>
@@ -6646,8 +6661,8 @@
       <c r="H16" s="26">
         <v>19.600000000000001</v>
       </c>
-      <c r="I16" s="27">
-        <v>2.3999999999999998E-7</v>
+      <c r="I16" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J16" s="27" t="s">
         <v>180</v>
@@ -6655,7 +6670,7 @@
       <c r="K16" s="26">
         <v>6.1</v>
       </c>
-      <c r="L16" s="27">
+      <c r="L16" s="49">
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="M16" s="27" t="s">
@@ -6669,8 +6684,8 @@
       <c r="B17" s="26">
         <v>198.3</v>
       </c>
-      <c r="C17" s="27">
-        <v>2.3999999999999998E-7</v>
+      <c r="C17" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D17" s="27" t="s">
         <v>180</v>
@@ -6678,8 +6693,8 @@
       <c r="E17" s="26">
         <v>16.8</v>
       </c>
-      <c r="F17" s="27">
-        <v>1.4000000000000001E-10</v>
+      <c r="F17" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="G17" s="27" t="s">
         <v>180</v>
@@ -6687,8 +6702,8 @@
       <c r="H17" s="26">
         <v>32.799999999999997</v>
       </c>
-      <c r="I17" s="27">
-        <v>2.3000000000000001E-10</v>
+      <c r="I17" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J17" s="27" t="s">
         <v>180</v>
@@ -6696,8 +6711,8 @@
       <c r="K17" s="26">
         <v>14.1</v>
       </c>
-      <c r="L17" s="27">
-        <v>7.8999999999999996E-10</v>
+      <c r="L17" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M17" s="27" t="s">
         <v>180</v>
@@ -6706,16 +6721,16 @@
     <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18" s="23"/>
       <c r="B18" s="26"/>
-      <c r="C18" s="27"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="27"/>
       <c r="E18" s="26"/>
-      <c r="F18" s="27"/>
+      <c r="F18" s="49"/>
       <c r="G18" s="27"/>
       <c r="H18" s="26"/>
-      <c r="I18" s="27"/>
+      <c r="I18" s="49"/>
       <c r="J18" s="27"/>
       <c r="K18" s="26"/>
-      <c r="L18" s="27"/>
+      <c r="L18" s="49"/>
       <c r="M18" s="27"/>
     </row>
     <row r="19" spans="1:13" ht="15" x14ac:dyDescent="0.15">
@@ -6723,16 +6738,16 @@
         <v>135</v>
       </c>
       <c r="B19" s="26"/>
-      <c r="C19" s="27"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="27"/>
       <c r="E19" s="26"/>
-      <c r="F19" s="27"/>
+      <c r="F19" s="49"/>
       <c r="G19" s="27"/>
       <c r="H19" s="26"/>
-      <c r="I19" s="27"/>
+      <c r="I19" s="49"/>
       <c r="J19" s="27"/>
       <c r="K19" s="26"/>
-      <c r="L19" s="27"/>
+      <c r="L19" s="49"/>
       <c r="M19" s="27"/>
     </row>
     <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.15">
@@ -6742,28 +6757,28 @@
       <c r="B20" s="26">
         <v>1.5</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20" s="49">
         <v>0.14000000000000001</v>
       </c>
       <c r="D20" s="27"/>
       <c r="E20" s="26">
         <v>1</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="49">
         <v>0.92</v>
       </c>
       <c r="G20" s="27"/>
       <c r="H20" s="26">
         <v>1.5</v>
       </c>
-      <c r="I20" s="27">
+      <c r="I20" s="49">
         <v>0.12</v>
       </c>
       <c r="J20" s="27"/>
       <c r="K20" s="26">
         <v>1.4</v>
       </c>
-      <c r="L20" s="27">
+      <c r="L20" s="49">
         <v>0.4</v>
       </c>
       <c r="M20" s="27"/>
@@ -6775,8 +6790,8 @@
       <c r="B21" s="26">
         <v>6.8</v>
       </c>
-      <c r="C21" s="27">
-        <v>3.3999999999999998E-32</v>
+      <c r="C21" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D21" s="27" t="s">
         <v>180</v>
@@ -6784,8 +6799,8 @@
       <c r="E21" s="26">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F21" s="27">
-        <v>1.5E-9</v>
+      <c r="F21" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="G21" s="27" t="s">
         <v>180</v>
@@ -6793,8 +6808,8 @@
       <c r="H21" s="26">
         <v>7.9</v>
       </c>
-      <c r="I21" s="27">
-        <v>2E-41</v>
+      <c r="I21" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J21" s="27" t="s">
         <v>180</v>
@@ -6802,8 +6817,8 @@
       <c r="K21" s="26">
         <v>8.1</v>
       </c>
-      <c r="L21" s="27">
-        <v>4.5999999999999998E-20</v>
+      <c r="L21" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M21" s="27" t="s">
         <v>180</v>
@@ -6816,8 +6831,8 @@
       <c r="B22" s="26">
         <v>5</v>
       </c>
-      <c r="C22" s="27">
-        <v>1.9000000000000001E-24</v>
+      <c r="C22" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D22" s="27" t="s">
         <v>180</v>
@@ -6825,8 +6840,8 @@
       <c r="E22" s="26">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F22" s="27">
-        <v>4.5999999999999998E-9</v>
+      <c r="F22" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="G22" s="27" t="s">
         <v>180</v>
@@ -6834,8 +6849,8 @@
       <c r="H22" s="26">
         <v>3.7</v>
       </c>
-      <c r="I22" s="27">
-        <v>3.1999999999999998E-19</v>
+      <c r="I22" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J22" s="27" t="s">
         <v>180</v>
@@ -6843,8 +6858,8 @@
       <c r="K22" s="26">
         <v>3.3</v>
       </c>
-      <c r="L22" s="27">
-        <v>8.0000000000000002E-8</v>
+      <c r="L22" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M22" s="27" t="s">
         <v>180</v>
@@ -6857,8 +6872,8 @@
       <c r="B23" s="26">
         <v>13.3</v>
       </c>
-      <c r="C23" s="27">
-        <v>4.6000000000000001E-32</v>
+      <c r="C23" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D23" s="27" t="s">
         <v>180</v>
@@ -6866,8 +6881,8 @@
       <c r="E23" s="26">
         <v>6.1</v>
       </c>
-      <c r="F23" s="27">
-        <v>6.3000000000000002E-9</v>
+      <c r="F23" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="G23" s="27" t="s">
         <v>180</v>
@@ -6875,8 +6890,8 @@
       <c r="H23" s="26">
         <v>6</v>
       </c>
-      <c r="I23" s="27">
-        <v>5.2999999999999998E-17</v>
+      <c r="I23" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J23" s="27" t="s">
         <v>180</v>
@@ -6884,8 +6899,8 @@
       <c r="K23" s="26">
         <v>5.8</v>
       </c>
-      <c r="L23" s="27">
-        <v>2.0000000000000001E-10</v>
+      <c r="L23" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M23" s="27" t="s">
         <v>180</v>
@@ -6898,8 +6913,8 @@
       <c r="B24" s="26">
         <v>18.5</v>
       </c>
-      <c r="C24" s="27">
-        <v>1.5E-24</v>
+      <c r="C24" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D24" s="27" t="s">
         <v>180</v>
@@ -6907,8 +6922,8 @@
       <c r="E24" s="26">
         <v>6.1</v>
       </c>
-      <c r="F24" s="27">
-        <v>1.3999999999999999E-6</v>
+      <c r="F24" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="G24" s="27" t="s">
         <v>180</v>
@@ -6916,8 +6931,8 @@
       <c r="H24" s="26">
         <v>8.9</v>
       </c>
-      <c r="I24" s="27">
-        <v>4.7000000000000004E-16</v>
+      <c r="I24" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J24" s="27" t="s">
         <v>180</v>
@@ -6925,8 +6940,8 @@
       <c r="K24" s="26">
         <v>7.4</v>
       </c>
-      <c r="L24" s="27">
-        <v>2.0000000000000001E-10</v>
+      <c r="L24" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M24" s="27" t="s">
         <v>180</v>
@@ -6939,8 +6954,8 @@
       <c r="B25" s="26">
         <v>12</v>
       </c>
-      <c r="C25" s="27">
-        <v>4.5999999999999998E-15</v>
+      <c r="C25" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D25" s="27" t="s">
         <v>180</v>
@@ -6948,7 +6963,7 @@
       <c r="E25" s="26">
         <v>5.4</v>
       </c>
-      <c r="F25" s="27">
+      <c r="F25" s="49">
         <v>1.1E-4</v>
       </c>
       <c r="G25" s="27" t="s">
@@ -6957,8 +6972,8 @@
       <c r="H25" s="26">
         <v>5.6</v>
       </c>
-      <c r="I25" s="27">
-        <v>2.6000000000000001E-8</v>
+      <c r="I25" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J25" s="27" t="s">
         <v>180</v>
@@ -6966,7 +6981,7 @@
       <c r="K25" s="26">
         <v>4.2</v>
       </c>
-      <c r="L25" s="27">
+      <c r="L25" s="49">
         <v>4.2000000000000002E-4</v>
       </c>
       <c r="M25" s="27" t="s">
@@ -6980,7 +6995,7 @@
       <c r="B26" s="26">
         <v>9.4</v>
       </c>
-      <c r="C26" s="27">
+      <c r="C26" s="49">
         <v>9.2000000000000003E-4</v>
       </c>
       <c r="D26" s="27" t="s">
@@ -6989,7 +7004,7 @@
       <c r="E26" s="26">
         <v>13.5</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F26" s="49">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="G26" s="27" t="s">
@@ -6998,7 +7013,7 @@
       <c r="H26" s="26">
         <v>11.8</v>
       </c>
-      <c r="I26" s="27">
+      <c r="I26" s="49">
         <v>5.1000000000000004E-4</v>
       </c>
       <c r="J26" s="27" t="s">
@@ -7007,8 +7022,8 @@
       <c r="K26" s="26">
         <v>15</v>
       </c>
-      <c r="L26" s="27">
-        <v>6.7999999999999999E-5</v>
+      <c r="L26" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M26" s="27" t="s">
         <v>180</v>
@@ -7021,8 +7036,8 @@
       <c r="B27" s="26">
         <v>12.7</v>
       </c>
-      <c r="C27" s="27">
-        <v>1.6999999999999999E-11</v>
+      <c r="C27" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D27" s="27" t="s">
         <v>180</v>
@@ -7030,7 +7045,7 @@
       <c r="E27" s="26">
         <v>4</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="49">
         <v>1.2E-2</v>
       </c>
       <c r="G27" s="27" t="s">
@@ -7039,8 +7054,8 @@
       <c r="H27" s="26">
         <v>7.5</v>
       </c>
-      <c r="I27" s="27">
-        <v>4.8E-8</v>
+      <c r="I27" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J27" s="27" t="s">
         <v>180</v>
@@ -7048,7 +7063,7 @@
       <c r="K27" s="26">
         <v>5.5</v>
       </c>
-      <c r="L27" s="27">
+      <c r="L27" s="49">
         <v>1.2999999999999999E-4</v>
       </c>
       <c r="M27" s="27" t="s">
@@ -7062,8 +7077,8 @@
       <c r="B28" s="26">
         <v>19.5</v>
       </c>
-      <c r="C28" s="27">
-        <v>6.3E-7</v>
+      <c r="C28" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D28" s="27" t="s">
         <v>180</v>
@@ -7071,14 +7086,14 @@
       <c r="E28" s="26">
         <v>4.5</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F28" s="49">
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="G28" s="27"/>
       <c r="H28" s="26">
         <v>4.5</v>
       </c>
-      <c r="I28" s="27">
+      <c r="I28" s="49">
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="J28" s="27" t="s">
@@ -7087,8 +7102,8 @@
       <c r="K28" s="26">
         <v>14.4</v>
       </c>
-      <c r="L28" s="27">
-        <v>1.3999999999999999E-6</v>
+      <c r="L28" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M28" s="27" t="s">
         <v>180</v>
@@ -7097,16 +7112,16 @@
     <row r="29" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A29" s="23"/>
       <c r="B29" s="26"/>
-      <c r="C29" s="27"/>
+      <c r="C29" s="49"/>
       <c r="D29" s="27"/>
       <c r="E29" s="26"/>
-      <c r="F29" s="27"/>
+      <c r="F29" s="49"/>
       <c r="G29" s="27"/>
       <c r="H29" s="26"/>
-      <c r="I29" s="27"/>
+      <c r="I29" s="49"/>
       <c r="J29" s="27"/>
       <c r="K29" s="26"/>
-      <c r="L29" s="27"/>
+      <c r="L29" s="49"/>
       <c r="M29" s="27"/>
     </row>
     <row r="30" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.15">
@@ -7114,16 +7129,16 @@
         <v>156</v>
       </c>
       <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
+      <c r="C30" s="48"/>
       <c r="D30" s="27"/>
       <c r="E30" s="26"/>
-      <c r="F30" s="27"/>
+      <c r="F30" s="49"/>
       <c r="G30" s="27"/>
       <c r="H30" s="26"/>
-      <c r="I30" s="27"/>
+      <c r="I30" s="49"/>
       <c r="J30" s="27"/>
       <c r="K30" s="26"/>
-      <c r="L30" s="27"/>
+      <c r="L30" s="49"/>
       <c r="M30" s="27"/>
     </row>
     <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.15">
@@ -7133,8 +7148,8 @@
       <c r="B31" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C31" s="27">
-        <v>5.9999999999999997E-15</v>
+      <c r="C31" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D31" s="27" t="s">
         <v>180</v>
@@ -7142,7 +7157,7 @@
       <c r="E31" s="26">
         <v>1</v>
       </c>
-      <c r="F31" s="27">
+      <c r="F31" s="49">
         <v>1.2E-4</v>
       </c>
       <c r="G31" s="27" t="s">
@@ -7151,8 +7166,8 @@
       <c r="H31" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I31" s="27">
-        <v>3.0999999999999999E-19</v>
+      <c r="I31" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J31" s="27" t="s">
         <v>180</v>
@@ -7160,8 +7175,8 @@
       <c r="K31" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L31" s="27">
-        <v>2.0000000000000001E-10</v>
+      <c r="L31" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M31" s="27" t="s">
         <v>180</v>
@@ -7174,7 +7189,7 @@
       <c r="B32" s="26">
         <v>1</v>
       </c>
-      <c r="C32" s="27">
+      <c r="C32" s="49">
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="D32" s="27" t="s">
@@ -7183,7 +7198,7 @@
       <c r="E32" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F32" s="27">
+      <c r="F32" s="49">
         <v>5.1999999999999995E-4</v>
       </c>
       <c r="G32" s="27" t="s">
@@ -7192,7 +7207,7 @@
       <c r="H32" s="26">
         <v>1</v>
       </c>
-      <c r="I32" s="27">
+      <c r="I32" s="49">
         <v>1.7000000000000001E-4</v>
       </c>
       <c r="J32" s="27" t="s">
@@ -7201,7 +7216,7 @@
       <c r="K32" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L32" s="27">
+      <c r="L32" s="49">
         <v>6.8999999999999997E-4</v>
       </c>
       <c r="M32" s="27" t="s">
@@ -7215,8 +7230,8 @@
       <c r="B33" s="26">
         <v>0.8</v>
       </c>
-      <c r="C33" s="27">
-        <v>3.4999999999999999E-6</v>
+      <c r="C33" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D33" s="27" t="s">
         <v>180</v>
@@ -7224,15 +7239,15 @@
       <c r="E33" s="26">
         <v>0.8</v>
       </c>
-      <c r="F33" s="27">
+      <c r="F33" s="49">
         <v>0.06</v>
       </c>
       <c r="G33" s="27"/>
       <c r="H33" s="26">
         <v>0.7</v>
       </c>
-      <c r="I33" s="27">
-        <v>6.1000000000000004E-8</v>
+      <c r="I33" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J33" s="27" t="s">
         <v>180</v>
@@ -7240,8 +7255,8 @@
       <c r="K33" s="26">
         <v>0.7</v>
       </c>
-      <c r="L33" s="27">
-        <v>5.3999999999999998E-5</v>
+      <c r="L33" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M33" s="27" t="s">
         <v>180</v>
@@ -7254,22 +7269,22 @@
       <c r="B34" s="26">
         <v>1</v>
       </c>
-      <c r="C34" s="27">
+      <c r="C34" s="49">
         <v>0.32</v>
       </c>
       <c r="D34" s="27"/>
       <c r="E34" s="26">
         <v>0.7</v>
       </c>
-      <c r="F34" s="27">
+      <c r="F34" s="49">
         <v>0.38</v>
       </c>
       <c r="G34" s="27"/>
       <c r="H34" s="26">
         <v>0.3</v>
       </c>
-      <c r="I34" s="27">
-        <v>3.7E-7</v>
+      <c r="I34" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J34" s="27" t="s">
         <v>180</v>
@@ -7277,7 +7292,7 @@
       <c r="K34" s="26">
         <v>0.4</v>
       </c>
-      <c r="L34" s="27">
+      <c r="L34" s="49">
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="M34" s="27" t="s">
@@ -7291,8 +7306,8 @@
       <c r="B35" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C35" s="27">
-        <v>8.0999999999999998E-12</v>
+      <c r="C35" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D35" s="27" t="s">
         <v>180</v>
@@ -7300,7 +7315,7 @@
       <c r="E35" s="26">
         <v>1</v>
       </c>
-      <c r="F35" s="27">
+      <c r="F35" s="49">
         <v>8.6999999999999994E-3</v>
       </c>
       <c r="G35" s="27" t="s">
@@ -7309,8 +7324,8 @@
       <c r="H35" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I35" s="27">
-        <v>1.2000000000000001E-19</v>
+      <c r="I35" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J35" s="27" t="s">
         <v>180</v>
@@ -7318,8 +7333,8 @@
       <c r="K35" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L35" s="27">
-        <v>3.0999999999999998E-17</v>
+      <c r="L35" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M35" s="27" t="s">
         <v>180</v>
@@ -7332,28 +7347,28 @@
       <c r="B36" s="26">
         <v>1</v>
       </c>
-      <c r="C36" s="27">
+      <c r="C36" s="49">
         <v>0.67</v>
       </c>
       <c r="D36" s="27"/>
       <c r="E36" s="26">
         <v>1</v>
       </c>
-      <c r="F36" s="27">
+      <c r="F36" s="49">
         <v>0.91</v>
       </c>
       <c r="G36" s="27"/>
       <c r="H36" s="26">
         <v>1</v>
       </c>
-      <c r="I36" s="27">
+      <c r="I36" s="49">
         <v>0.45</v>
       </c>
       <c r="J36" s="27"/>
       <c r="K36" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L36" s="27">
+      <c r="L36" s="49">
         <v>0.02</v>
       </c>
       <c r="M36" s="27" t="s">
@@ -7367,7 +7382,7 @@
       <c r="B37" s="26">
         <v>1</v>
       </c>
-      <c r="C37" s="27">
+      <c r="C37" s="49">
         <v>8.3999999999999995E-3</v>
       </c>
       <c r="D37" s="27" t="s">
@@ -7376,15 +7391,15 @@
       <c r="E37" s="26">
         <v>1</v>
       </c>
-      <c r="F37" s="27">
+      <c r="F37" s="49">
         <v>0.84</v>
       </c>
       <c r="G37" s="27"/>
       <c r="H37" s="26">
         <v>1</v>
       </c>
-      <c r="I37" s="27">
-        <v>9.3999999999999994E-5</v>
+      <c r="I37" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J37" s="27" t="s">
         <v>180</v>
@@ -7392,8 +7407,8 @@
       <c r="K37" s="26">
         <v>1</v>
       </c>
-      <c r="L37" s="27">
-        <v>9.7000000000000003E-6</v>
+      <c r="L37" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M37" s="27" t="s">
         <v>180</v>
@@ -7406,7 +7421,7 @@
       <c r="B38" s="26">
         <v>1</v>
       </c>
-      <c r="C38" s="27">
+      <c r="C38" s="49">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="D38" s="27" t="s">
@@ -7415,15 +7430,15 @@
       <c r="E38" s="26">
         <v>1</v>
       </c>
-      <c r="F38" s="27">
+      <c r="F38" s="49">
         <v>0.8</v>
       </c>
       <c r="G38" s="27"/>
       <c r="H38" s="26">
         <v>1</v>
       </c>
-      <c r="I38" s="27">
-        <v>1.5E-6</v>
+      <c r="I38" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J38" s="27" t="s">
         <v>180</v>
@@ -7431,8 +7446,8 @@
       <c r="K38" s="26">
         <v>1</v>
       </c>
-      <c r="L38" s="27">
-        <v>3E-10</v>
+      <c r="L38" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="M38" s="27" t="s">
         <v>180</v>
@@ -7443,16 +7458,16 @@
         <v>171</v>
       </c>
       <c r="B39" s="26"/>
-      <c r="C39" s="27"/>
+      <c r="C39" s="49"/>
       <c r="D39" s="27"/>
       <c r="E39" s="26"/>
-      <c r="F39" s="27"/>
+      <c r="F39" s="49"/>
       <c r="G39" s="27"/>
       <c r="H39" s="26"/>
-      <c r="I39" s="27"/>
+      <c r="I39" s="49"/>
       <c r="J39" s="27"/>
       <c r="K39" s="26"/>
-      <c r="L39" s="27"/>
+      <c r="L39" s="49"/>
       <c r="M39" s="27"/>
     </row>
     <row r="40" spans="1:13" ht="15" x14ac:dyDescent="0.15">
@@ -7462,21 +7477,21 @@
       <c r="B40" s="26">
         <v>1</v>
       </c>
-      <c r="C40" s="27">
+      <c r="C40" s="49">
         <v>0.12</v>
       </c>
       <c r="D40" s="27"/>
       <c r="E40" s="26">
         <v>1</v>
       </c>
-      <c r="F40" s="27">
+      <c r="F40" s="49">
         <v>0.53</v>
       </c>
       <c r="G40" s="27"/>
       <c r="H40" s="26">
         <v>1</v>
       </c>
-      <c r="I40" s="27">
+      <c r="I40" s="49">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="J40" s="27" t="s">
@@ -7485,7 +7500,7 @@
       <c r="K40" s="26">
         <v>1</v>
       </c>
-      <c r="L40" s="27">
+      <c r="L40" s="49">
         <v>0.12</v>
       </c>
       <c r="M40" s="27"/>
@@ -7497,28 +7512,28 @@
       <c r="B41" s="26">
         <v>1</v>
       </c>
-      <c r="C41" s="27">
+      <c r="C41" s="49">
         <v>0.7</v>
       </c>
       <c r="D41" s="27"/>
       <c r="E41" s="26">
         <v>1</v>
       </c>
-      <c r="F41" s="27">
+      <c r="F41" s="49">
         <v>0.56999999999999995</v>
       </c>
       <c r="G41" s="27"/>
       <c r="H41" s="26">
         <v>1</v>
       </c>
-      <c r="I41" s="27">
+      <c r="I41" s="49">
         <v>0.33</v>
       </c>
       <c r="J41" s="27"/>
       <c r="K41" s="26">
         <v>1</v>
       </c>
-      <c r="L41" s="27">
+      <c r="L41" s="49">
         <v>0.79</v>
       </c>
       <c r="M41" s="27"/>
@@ -7530,7 +7545,7 @@
       <c r="B42" s="26">
         <v>1</v>
       </c>
-      <c r="C42" s="27">
+      <c r="C42" s="49">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="D42" s="27" t="s">
@@ -7539,7 +7554,7 @@
       <c r="E42" s="26">
         <v>1</v>
       </c>
-      <c r="F42" s="27">
+      <c r="F42" s="49">
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="G42" s="27" t="s">
@@ -7548,7 +7563,7 @@
       <c r="H42" s="26">
         <v>1</v>
       </c>
-      <c r="I42" s="27">
+      <c r="I42" s="49">
         <v>1.6E-2</v>
       </c>
       <c r="J42" s="27" t="s">
@@ -7557,7 +7572,7 @@
       <c r="K42" s="26">
         <v>1</v>
       </c>
-      <c r="L42" s="27">
+      <c r="L42" s="49">
         <v>0.76</v>
       </c>
       <c r="M42" s="27"/>
@@ -7569,28 +7584,28 @@
       <c r="B43" s="26">
         <v>1</v>
       </c>
-      <c r="C43" s="27">
+      <c r="C43" s="49">
         <v>0.44</v>
       </c>
       <c r="D43" s="27"/>
       <c r="E43" s="26">
         <v>1</v>
       </c>
-      <c r="F43" s="27">
+      <c r="F43" s="49">
         <v>0.26</v>
       </c>
       <c r="G43" s="27"/>
       <c r="H43" s="26">
         <v>1</v>
       </c>
-      <c r="I43" s="27">
+      <c r="I43" s="49">
         <v>0.79</v>
       </c>
       <c r="J43" s="27"/>
       <c r="K43" s="26">
         <v>1</v>
       </c>
-      <c r="L43" s="27">
+      <c r="L43" s="49">
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="M43" s="27"/>
@@ -7602,28 +7617,28 @@
       <c r="B44" s="26">
         <v>1</v>
       </c>
-      <c r="C44" s="27">
+      <c r="C44" s="49">
         <v>0.83</v>
       </c>
       <c r="D44" s="27"/>
       <c r="E44" s="26">
         <v>1</v>
       </c>
-      <c r="F44" s="27">
+      <c r="F44" s="49">
         <v>0.75</v>
       </c>
       <c r="G44" s="27"/>
       <c r="H44" s="26">
         <v>0.9</v>
       </c>
-      <c r="I44" s="27">
+      <c r="I44" s="49">
         <v>0.19</v>
       </c>
       <c r="J44" s="27"/>
       <c r="K44" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L44" s="27">
+      <c r="L44" s="49">
         <v>0.42</v>
       </c>
       <c r="M44" s="27"/>
@@ -7635,21 +7650,21 @@
       <c r="B45" s="26">
         <v>0.9</v>
       </c>
-      <c r="C45" s="27">
+      <c r="C45" s="49">
         <v>0.34</v>
       </c>
       <c r="D45" s="27"/>
       <c r="E45" s="26">
         <v>0.8</v>
       </c>
-      <c r="F45" s="27">
+      <c r="F45" s="49">
         <v>0.35</v>
       </c>
       <c r="G45" s="27"/>
       <c r="H45" s="26">
         <v>0.8</v>
       </c>
-      <c r="I45" s="27">
+      <c r="I45" s="49">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="J45" s="27" t="s">
@@ -7658,7 +7673,7 @@
       <c r="K45" s="26">
         <v>1</v>
       </c>
-      <c r="L45" s="27">
+      <c r="L45" s="49">
         <v>0.83</v>
       </c>
       <c r="M45" s="27"/>
@@ -7670,28 +7685,28 @@
       <c r="B46" s="26">
         <v>1</v>
       </c>
-      <c r="C46" s="27">
+      <c r="C46" s="49">
         <v>0.76</v>
       </c>
       <c r="D46" s="27"/>
       <c r="E46" s="26">
         <v>1</v>
       </c>
-      <c r="F46" s="27">
+      <c r="F46" s="49">
         <v>0.97</v>
       </c>
       <c r="G46" s="27"/>
       <c r="H46" s="26">
         <v>0.9</v>
       </c>
-      <c r="I46" s="27">
+      <c r="I46" s="49">
         <v>0.13</v>
       </c>
       <c r="J46" s="27"/>
       <c r="K46" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L46" s="27">
+      <c r="L46" s="49">
         <v>0.36</v>
       </c>
       <c r="M46" s="27"/>
@@ -7703,28 +7718,28 @@
       <c r="B47" s="26">
         <v>1</v>
       </c>
-      <c r="C47" s="27">
+      <c r="C47" s="49">
         <v>0.96</v>
       </c>
       <c r="D47" s="27"/>
       <c r="E47" s="26">
         <v>1</v>
       </c>
-      <c r="F47" s="27">
+      <c r="F47" s="49">
         <v>0.86</v>
       </c>
       <c r="G47" s="27"/>
       <c r="H47" s="26">
         <v>0.9</v>
       </c>
-      <c r="I47" s="27">
+      <c r="I47" s="49">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="J47" s="27"/>
       <c r="K47" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L47" s="27">
+      <c r="L47" s="49">
         <v>0.2</v>
       </c>
       <c r="M47" s="27"/>
@@ -7732,16 +7747,24 @@
     <row r="48" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A48" s="23"/>
       <c r="B48" s="26"/>
-      <c r="C48" s="27"/>
+      <c r="C48" s="49" t="s">
+        <v>322</v>
+      </c>
       <c r="D48" s="27"/>
       <c r="E48" s="26"/>
-      <c r="F48" s="27"/>
+      <c r="F48" s="49" t="s">
+        <v>322</v>
+      </c>
       <c r="G48" s="27"/>
       <c r="H48" s="26"/>
-      <c r="I48" s="27"/>
+      <c r="I48" s="49" t="s">
+        <v>322</v>
+      </c>
       <c r="J48" s="27"/>
       <c r="K48" s="26"/>
-      <c r="L48" s="27"/>
+      <c r="L48" s="49" t="s">
+        <v>322</v>
+      </c>
       <c r="M48" s="27"/>
     </row>
     <row r="49" spans="1:13" ht="15" x14ac:dyDescent="0.15">
@@ -7749,16 +7772,24 @@
         <v>181</v>
       </c>
       <c r="B49" s="26"/>
-      <c r="C49" s="27"/>
+      <c r="C49" s="49" t="s">
+        <v>322</v>
+      </c>
       <c r="D49" s="27"/>
       <c r="E49" s="26"/>
-      <c r="F49" s="27"/>
+      <c r="F49" s="49" t="s">
+        <v>322</v>
+      </c>
       <c r="G49" s="27"/>
       <c r="H49" s="26"/>
-      <c r="I49" s="27"/>
+      <c r="I49" s="49" t="s">
+        <v>322</v>
+      </c>
       <c r="J49" s="27"/>
       <c r="K49" s="26"/>
-      <c r="L49" s="27"/>
+      <c r="L49" s="49" t="s">
+        <v>322</v>
+      </c>
       <c r="M49" s="27"/>
     </row>
     <row r="50" spans="1:13" ht="15" x14ac:dyDescent="0.15">
@@ -7768,7 +7799,7 @@
       <c r="B50" s="26">
         <v>0.5</v>
       </c>
-      <c r="C50" s="27">
+      <c r="C50" s="49">
         <v>8.4000000000000003E-4</v>
       </c>
       <c r="D50" s="27" t="s">
@@ -7777,15 +7808,15 @@
       <c r="E50" s="26">
         <v>0.7</v>
       </c>
-      <c r="F50" s="27">
+      <c r="F50" s="49">
         <v>0.17</v>
       </c>
       <c r="G50" s="27"/>
       <c r="H50" s="26">
         <v>0.5</v>
       </c>
-      <c r="I50" s="27">
-        <v>9.2999999999999997E-5</v>
+      <c r="I50" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J50" s="27" t="s">
         <v>180</v>
@@ -7793,7 +7824,7 @@
       <c r="K50" s="26">
         <v>0.5</v>
       </c>
-      <c r="L50" s="27">
+      <c r="L50" s="49">
         <v>0.02</v>
       </c>
       <c r="M50" s="27" t="s">
@@ -7807,28 +7838,28 @@
       <c r="B51" s="26">
         <v>1</v>
       </c>
-      <c r="C51" s="27">
+      <c r="C51" s="49">
         <v>0.79</v>
       </c>
       <c r="D51" s="27"/>
       <c r="E51" s="26">
         <v>1</v>
       </c>
-      <c r="F51" s="27">
+      <c r="F51" s="49">
         <v>0.93</v>
       </c>
       <c r="G51" s="27"/>
       <c r="H51" s="26">
         <v>0.8</v>
       </c>
-      <c r="I51" s="27">
+      <c r="I51" s="49">
         <v>0.24</v>
       </c>
       <c r="J51" s="27"/>
       <c r="K51" s="26">
         <v>0.8</v>
       </c>
-      <c r="L51" s="27">
+      <c r="L51" s="49">
         <v>0.26</v>
       </c>
       <c r="M51" s="27"/>
@@ -7840,8 +7871,8 @@
       <c r="B52" s="26">
         <v>0.4</v>
       </c>
-      <c r="C52" s="27">
-        <v>1.2999999999999999E-5</v>
+      <c r="C52" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D52" s="27" t="s">
         <v>180</v>
@@ -7849,7 +7880,7 @@
       <c r="E52" s="26">
         <v>0.5</v>
       </c>
-      <c r="F52" s="27">
+      <c r="F52" s="49">
         <v>0.04</v>
       </c>
       <c r="G52" s="27" t="s">
@@ -7858,8 +7889,8 @@
       <c r="H52" s="26">
         <v>0.2</v>
       </c>
-      <c r="I52" s="27">
-        <v>5.2999999999999998E-11</v>
+      <c r="I52" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J52" s="27" t="s">
         <v>180</v>
@@ -7867,7 +7898,7 @@
       <c r="K52" s="26">
         <v>0.3</v>
       </c>
-      <c r="L52" s="27">
+      <c r="L52" s="49">
         <v>3.6000000000000002E-4</v>
       </c>
       <c r="M52" s="27" t="s">
@@ -7881,14 +7912,14 @@
       <c r="B53" s="26">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C53" s="27">
+      <c r="C53" s="49">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D53" s="27"/>
       <c r="E53" s="26">
         <v>3.5</v>
       </c>
-      <c r="F53" s="27">
+      <c r="F53" s="49">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="G53" s="27" t="s">
@@ -7897,14 +7928,14 @@
       <c r="H53" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I53" s="27">
+      <c r="I53" s="49">
         <v>0.87</v>
       </c>
       <c r="J53" s="27"/>
       <c r="K53" s="26">
         <v>2.5</v>
       </c>
-      <c r="L53" s="27">
+      <c r="L53" s="49">
         <v>0.15</v>
       </c>
       <c r="M53" s="27"/>
@@ -7916,136 +7947,148 @@
       <c r="B54" s="26">
         <v>2.6</v>
       </c>
-      <c r="C54" s="27">
+      <c r="C54" s="49">
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="D54" s="27"/>
       <c r="E54" s="26">
         <v>0</v>
       </c>
-      <c r="F54" s="27">
+      <c r="F54" s="49">
         <v>0.98</v>
       </c>
       <c r="G54" s="27"/>
       <c r="H54" s="26">
         <v>2.1</v>
       </c>
-      <c r="I54" s="27">
+      <c r="I54" s="49">
         <v>0.17</v>
       </c>
       <c r="J54" s="27"/>
       <c r="K54" s="26">
         <v>2.1</v>
       </c>
-      <c r="L54" s="27">
+      <c r="L54" s="49">
         <v>0.33</v>
       </c>
       <c r="M54" s="27"/>
     </row>
-    <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A55" s="25" t="s">
-        <v>79</v>
+        <v>201</v>
       </c>
       <c r="B55" s="26">
-        <v>0</v>
-      </c>
-      <c r="C55" s="27">
-        <v>0.98</v>
-      </c>
-      <c r="D55" s="27"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C55" s="49">
+        <v>3.9E-2</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>180</v>
+      </c>
       <c r="E55" s="26">
-        <v>0</v>
-      </c>
-      <c r="F55" s="27">
-        <v>0.99</v>
-      </c>
-      <c r="G55" s="27"/>
+        <v>3</v>
+      </c>
+      <c r="F55" s="49">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G55" s="27" t="s">
+        <v>180</v>
+      </c>
       <c r="H55" s="26">
-        <v>0.6</v>
-      </c>
-      <c r="I55" s="27">
-        <v>0.67</v>
+        <v>1.3</v>
+      </c>
+      <c r="I55" s="49">
+        <v>0.57999999999999996</v>
       </c>
       <c r="J55" s="27"/>
       <c r="K55" s="26">
-        <v>0</v>
-      </c>
-      <c r="L55" s="27">
-        <v>0.98</v>
-      </c>
-      <c r="M55" s="27"/>
-    </row>
-    <row r="56" spans="1:13" ht="30" x14ac:dyDescent="0.15">
+        <v>2.7</v>
+      </c>
+      <c r="L55" s="49">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="M55" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A56" s="25" t="s">
-        <v>80</v>
+        <v>182</v>
       </c>
       <c r="B56" s="26">
-        <v>2.9</v>
-      </c>
-      <c r="C56" s="27">
-        <v>0.2</v>
-      </c>
-      <c r="D56" s="27"/>
+        <v>6.4</v>
+      </c>
+      <c r="C56" s="49" t="s">
+        <v>322</v>
+      </c>
+      <c r="D56" s="27" t="s">
+        <v>180</v>
+      </c>
       <c r="E56" s="26">
-        <v>10.3</v>
-      </c>
-      <c r="F56" s="27">
-        <v>5.8999999999999999E-3</v>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F56" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="G56" s="27" t="s">
         <v>180</v>
       </c>
       <c r="H56" s="26">
-        <v>7.8</v>
-      </c>
-      <c r="I56" s="27">
-        <v>7.6E-3</v>
+        <v>3.6</v>
+      </c>
+      <c r="I56" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J56" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K56" s="26">
-        <v>3</v>
-      </c>
-      <c r="L56" s="27">
-        <v>0.32</v>
-      </c>
-      <c r="M56" s="27"/>
+        <v>3.6</v>
+      </c>
+      <c r="L56" s="49" t="s">
+        <v>322</v>
+      </c>
+      <c r="M56" s="27" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="57" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A57" s="25" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B57" s="26">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C57" s="27">
-        <v>3.9E-2</v>
+        <v>3.8</v>
+      </c>
+      <c r="C57" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D57" s="27" t="s">
         <v>180</v>
       </c>
       <c r="E57" s="26">
-        <v>3</v>
-      </c>
-      <c r="F57" s="27">
-        <v>4.4999999999999998E-2</v>
+        <v>2.7</v>
+      </c>
+      <c r="F57" s="49">
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="G57" s="27" t="s">
         <v>180</v>
       </c>
       <c r="H57" s="26">
-        <v>1.3</v>
-      </c>
-      <c r="I57" s="27">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="J57" s="27"/>
+        <v>3.4</v>
+      </c>
+      <c r="I57" s="49" t="s">
+        <v>322</v>
+      </c>
+      <c r="J57" s="27" t="s">
+        <v>180</v>
+      </c>
       <c r="K57" s="26">
-        <v>2.7</v>
-      </c>
-      <c r="L57" s="27">
-        <v>4.3999999999999997E-2</v>
+        <v>3.4</v>
+      </c>
+      <c r="L57" s="49">
+        <v>1.7000000000000001E-4</v>
       </c>
       <c r="M57" s="27" t="s">
         <v>180</v>
@@ -8053,40 +8096,38 @@
     </row>
     <row r="58" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A58" s="25" t="s">
-        <v>182</v>
+        <v>81</v>
       </c>
       <c r="B58" s="26">
-        <v>6.4</v>
-      </c>
-      <c r="C58" s="27">
-        <v>1.5E-19</v>
+        <v>3.3</v>
+      </c>
+      <c r="C58" s="49">
+        <v>2.7E-2</v>
       </c>
       <c r="D58" s="27" t="s">
         <v>180</v>
       </c>
       <c r="E58" s="26">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="F58" s="27">
-        <v>2.3999999999999999E-6</v>
-      </c>
-      <c r="G58" s="27" t="s">
-        <v>180</v>
-      </c>
+        <v>1.7</v>
+      </c>
+      <c r="F58" s="49">
+        <v>0.62</v>
+      </c>
+      <c r="G58" s="27"/>
       <c r="H58" s="26">
-        <v>3.6</v>
-      </c>
-      <c r="I58" s="27">
-        <v>3.1000000000000002E-10</v>
+        <v>3.5</v>
+      </c>
+      <c r="I58" s="49">
+        <v>1.6E-2</v>
       </c>
       <c r="J58" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K58" s="26">
-        <v>3.6</v>
-      </c>
-      <c r="L58" s="27">
-        <v>5.6999999999999996E-6</v>
+        <v>4.2</v>
+      </c>
+      <c r="L58" s="49">
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="M58" s="27" t="s">
         <v>180</v>
@@ -8094,381 +8135,301 @@
     </row>
     <row r="59" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A59" s="25" t="s">
-        <v>199</v>
+        <v>71</v>
       </c>
       <c r="B59" s="26">
-        <v>3.8</v>
-      </c>
-      <c r="C59" s="27">
-        <v>4.6999999999999997E-8</v>
+        <v>2.8</v>
+      </c>
+      <c r="C59" s="49">
+        <v>2E-3</v>
       </c>
       <c r="D59" s="27" t="s">
         <v>180</v>
       </c>
       <c r="E59" s="26">
-        <v>2.7</v>
-      </c>
-      <c r="F59" s="27">
-        <v>1.0999999999999999E-2</v>
+        <v>5.7</v>
+      </c>
+      <c r="F59" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="G59" s="27" t="s">
         <v>180</v>
       </c>
       <c r="H59" s="26">
-        <v>3.4</v>
-      </c>
-      <c r="I59" s="27">
-        <v>2.2999999999999999E-7</v>
+        <v>4</v>
+      </c>
+      <c r="I59" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J59" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K59" s="26">
-        <v>3.4</v>
-      </c>
-      <c r="L59" s="27">
-        <v>1.7000000000000001E-4</v>
-      </c>
-      <c r="M59" s="27" t="s">
-        <v>180</v>
-      </c>
+        <v>1.6</v>
+      </c>
+      <c r="L59" s="49">
+        <v>0.36</v>
+      </c>
+      <c r="M59" s="27"/>
     </row>
     <row r="60" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A60" s="25" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B60" s="26">
-        <v>3.3</v>
-      </c>
-      <c r="C60" s="27">
-        <v>2.7E-2</v>
+        <v>3.7</v>
+      </c>
+      <c r="C60" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="D60" s="27" t="s">
         <v>180</v>
       </c>
       <c r="E60" s="26">
-        <v>1.7</v>
-      </c>
-      <c r="F60" s="27">
-        <v>0.62</v>
+        <v>1.9</v>
+      </c>
+      <c r="F60" s="49">
+        <v>0.28999999999999998</v>
       </c>
       <c r="G60" s="27"/>
       <c r="H60" s="26">
-        <v>3.5</v>
-      </c>
-      <c r="I60" s="27">
-        <v>1.6E-2</v>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I60" s="49" t="s">
+        <v>322</v>
       </c>
       <c r="J60" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K60" s="26">
-        <v>4.2</v>
-      </c>
-      <c r="L60" s="27">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="M60" s="27" t="s">
-        <v>180</v>
-      </c>
+        <v>2.4</v>
+      </c>
+      <c r="L60" s="49">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="M60" s="27"/>
     </row>
     <row r="61" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A61" s="25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B61" s="26">
-        <v>2.8</v>
-      </c>
-      <c r="C61" s="27">
-        <v>2E-3</v>
+        <v>2.5</v>
+      </c>
+      <c r="C61" s="49">
+        <v>1.4E-3</v>
       </c>
       <c r="D61" s="27" t="s">
         <v>180</v>
       </c>
       <c r="E61" s="26">
-        <v>5.7</v>
-      </c>
-      <c r="F61" s="27">
-        <v>2.3E-5</v>
-      </c>
-      <c r="G61" s="27" t="s">
-        <v>180</v>
-      </c>
+        <v>1.5</v>
+      </c>
+      <c r="F61" s="49">
+        <v>0.48</v>
+      </c>
+      <c r="G61" s="27"/>
       <c r="H61" s="26">
-        <v>4</v>
-      </c>
-      <c r="I61" s="27">
-        <v>5.3000000000000001E-6</v>
+        <v>2.7</v>
+      </c>
+      <c r="I61" s="49">
+        <v>1.1E-4</v>
       </c>
       <c r="J61" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K61" s="26">
-        <v>1.6</v>
-      </c>
-      <c r="L61" s="27">
-        <v>0.36</v>
-      </c>
-      <c r="M61" s="27"/>
+        <v>2.6</v>
+      </c>
+      <c r="L61" s="49">
+        <v>0.01</v>
+      </c>
+      <c r="M61" s="27" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="62" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A62" s="25" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B62" s="26">
-        <v>3.7</v>
-      </c>
-      <c r="C62" s="27">
-        <v>9.7999999999999997E-5</v>
-      </c>
-      <c r="D62" s="27" t="s">
-        <v>180</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C62" s="49">
+        <v>0.98</v>
+      </c>
+      <c r="D62" s="27"/>
       <c r="E62" s="26">
-        <v>1.9</v>
-      </c>
-      <c r="F62" s="27">
-        <v>0.28999999999999998</v>
+        <v>0</v>
+      </c>
+      <c r="F62" s="49">
+        <v>0.98</v>
       </c>
       <c r="G62" s="27"/>
       <c r="H62" s="26">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="I62" s="27">
-        <v>3.3000000000000002E-6</v>
-      </c>
-      <c r="J62" s="27" t="s">
-        <v>180</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I62" s="49">
+        <v>0.97</v>
+      </c>
+      <c r="J62" s="27"/>
       <c r="K62" s="26">
-        <v>2.4</v>
-      </c>
-      <c r="L62" s="27">
-        <v>7.3999999999999996E-2</v>
+        <v>0</v>
+      </c>
+      <c r="L62" s="49">
+        <v>0.98</v>
       </c>
       <c r="M62" s="27"/>
     </row>
     <row r="63" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A63" s="25" t="s">
-        <v>69</v>
+        <v>183</v>
       </c>
       <c r="B63" s="26">
-        <v>2.5</v>
-      </c>
-      <c r="C63" s="27">
-        <v>1.4E-3</v>
+        <v>2.4</v>
+      </c>
+      <c r="C63" s="49">
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="D63" s="27" t="s">
         <v>180</v>
       </c>
       <c r="E63" s="26">
-        <v>1.5</v>
-      </c>
-      <c r="F63" s="27">
-        <v>0.48</v>
+        <v>1.6</v>
+      </c>
+      <c r="F63" s="49">
+        <v>0.31</v>
       </c>
       <c r="G63" s="27"/>
       <c r="H63" s="26">
-        <v>2.7</v>
-      </c>
-      <c r="I63" s="27">
-        <v>1.1E-4</v>
+        <v>2</v>
+      </c>
+      <c r="I63" s="49">
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="J63" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K63" s="26">
-        <v>2.6</v>
-      </c>
-      <c r="L63" s="27">
-        <v>0.01</v>
-      </c>
-      <c r="M63" s="27" t="s">
-        <v>180</v>
-      </c>
+        <v>1.7</v>
+      </c>
+      <c r="L63" s="49">
+        <v>0.22</v>
+      </c>
+      <c r="M63" s="27"/>
     </row>
     <row r="64" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A64" s="25" t="s">
-        <v>76</v>
+        <v>184</v>
       </c>
       <c r="B64" s="26">
-        <v>0</v>
-      </c>
-      <c r="C64" s="27">
-        <v>0.98</v>
-      </c>
-      <c r="D64" s="27"/>
+        <v>2.1</v>
+      </c>
+      <c r="C64" s="49">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="D64" s="27" t="s">
+        <v>180</v>
+      </c>
       <c r="E64" s="26">
-        <v>0</v>
-      </c>
-      <c r="F64" s="27">
-        <v>0.98</v>
+        <v>1.9</v>
+      </c>
+      <c r="F64" s="49">
+        <v>0.14000000000000001</v>
       </c>
       <c r="G64" s="27"/>
       <c r="H64" s="26">
-        <v>0</v>
-      </c>
-      <c r="I64" s="27">
-        <v>0.97</v>
-      </c>
-      <c r="J64" s="27"/>
+        <v>1.8</v>
+      </c>
+      <c r="I64" s="49">
+        <v>1.9E-2</v>
+      </c>
+      <c r="J64" s="27" t="s">
+        <v>180</v>
+      </c>
       <c r="K64" s="26">
-        <v>0</v>
-      </c>
-      <c r="L64" s="27">
-        <v>0.98</v>
+        <v>1.3</v>
+      </c>
+      <c r="L64" s="49">
+        <v>0.56000000000000005</v>
       </c>
       <c r="M64" s="27"/>
     </row>
     <row r="65" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A65" s="25" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="B65" s="26">
-        <v>2.4</v>
-      </c>
-      <c r="C65" s="27">
-        <v>1.1000000000000001E-3</v>
+        <v>4.7</v>
+      </c>
+      <c r="C65" s="49">
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="D65" s="27" t="s">
         <v>180</v>
       </c>
       <c r="E65" s="26">
-        <v>1.6</v>
-      </c>
-      <c r="F65" s="27">
-        <v>0.31</v>
-      </c>
-      <c r="G65" s="27"/>
+        <v>6.4</v>
+      </c>
+      <c r="F65" s="49">
+        <v>3.2000000000000003E-4</v>
+      </c>
+      <c r="G65" s="27" t="s">
+        <v>180</v>
+      </c>
       <c r="H65" s="26">
-        <v>2</v>
-      </c>
-      <c r="I65" s="27">
-        <v>8.3999999999999995E-3</v>
-      </c>
-      <c r="J65" s="27" t="s">
-        <v>180</v>
-      </c>
+        <v>2.1</v>
+      </c>
+      <c r="I65" s="49">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="J65" s="27"/>
       <c r="K65" s="26">
-        <v>1.7</v>
-      </c>
-      <c r="L65" s="27">
-        <v>0.22</v>
-      </c>
-      <c r="M65" s="27"/>
+        <v>3.3</v>
+      </c>
+      <c r="L65" s="49">
+        <v>3.1E-2</v>
+      </c>
+      <c r="M65" s="27" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="66" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A66" s="25" t="s">
-        <v>184</v>
+        <v>74</v>
       </c>
       <c r="B66" s="26">
-        <v>2.1</v>
-      </c>
-      <c r="C66" s="27">
-        <v>7.3000000000000001E-3</v>
+        <v>3.2</v>
+      </c>
+      <c r="C66" s="49">
+        <v>0.01</v>
       </c>
       <c r="D66" s="27" t="s">
         <v>180</v>
       </c>
       <c r="E66" s="26">
-        <v>1.9</v>
-      </c>
-      <c r="F66" s="27">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G66" s="27"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F66" s="49">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="G66" s="27" t="s">
+        <v>180</v>
+      </c>
       <c r="H66" s="26">
+        <v>1.7</v>
+      </c>
+      <c r="I66" s="49">
+        <v>0.3</v>
+      </c>
+      <c r="J66" s="27"/>
+      <c r="K66" s="26">
         <v>1.8</v>
       </c>
-      <c r="I66" s="27">
-        <v>1.9E-2</v>
-      </c>
-      <c r="J66" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K66" s="26">
-        <v>1.3</v>
-      </c>
-      <c r="L66" s="27">
-        <v>0.56000000000000005</v>
+      <c r="L66" s="49">
+        <v>0.44</v>
       </c>
       <c r="M66" s="27"/>
-    </row>
-    <row r="67" spans="1:13" ht="15" x14ac:dyDescent="0.15">
-      <c r="A67" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="B67" s="26">
-        <v>4.7</v>
-      </c>
-      <c r="C67" s="27">
-        <v>1.6000000000000001E-4</v>
-      </c>
-      <c r="D67" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="E67" s="26">
-        <v>6.4</v>
-      </c>
-      <c r="F67" s="27">
-        <v>3.2000000000000003E-4</v>
-      </c>
-      <c r="G67" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="H67" s="26">
-        <v>2.1</v>
-      </c>
-      <c r="I67" s="27">
-        <v>8.8999999999999996E-2</v>
-      </c>
-      <c r="J67" s="27"/>
-      <c r="K67" s="26">
-        <v>3.3</v>
-      </c>
-      <c r="L67" s="27">
-        <v>3.1E-2</v>
-      </c>
-      <c r="M67" s="27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" ht="15" x14ac:dyDescent="0.15">
-      <c r="A68" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="B68" s="26">
-        <v>3.2</v>
-      </c>
-      <c r="C68" s="27">
-        <v>0.01</v>
-      </c>
-      <c r="D68" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="E68" s="26">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F68" s="27">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="G68" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="H68" s="26">
-        <v>1.7</v>
-      </c>
-      <c r="I68" s="27">
-        <v>0.3</v>
-      </c>
-      <c r="J68" s="27"/>
-      <c r="K68" s="26">
-        <v>1.8</v>
-      </c>
-      <c r="L68" s="27">
-        <v>0.44</v>
-      </c>
-      <c r="M68" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -10491,7 +10452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1880468A-055E-BA41-A377-B9D926328429}">
   <dimension ref="A1:P109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F41" workbookViewId="0">
+    <sheetView topLeftCell="F41" workbookViewId="0">
       <selection activeCell="P63" sqref="P63"/>
     </sheetView>
   </sheetViews>

</xml_diff>